<commit_message>
Tweaks to settings tool.
</commit_message>
<xml_diff>
--- a/tools/CoMet_Settings_Tool.xlsx
+++ b/tools/CoMet_Settings_Tool.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjd/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjd/Desktop/DESKTOP_FILES/Genomics/genomics_gpu/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E335333-CB1B-5640-8DC9-AF0F0354BBBC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3608401F-6CFB-464F-81CE-AABBCCCC67ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="620" windowWidth="26520" windowHeight="26480" xr2:uid="{FA80413B-B473-9946-BFAA-BCC79B485766}"/>
   </bookViews>
@@ -1935,9 +1935,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1953,7 +1953,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6540500" y="5740400"/>
-          <a:ext cx="5727700" cy="4432300"/>
+          <a:ext cx="5981700" cy="4686300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2006,7 +2006,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>- settings are set acceptably when ALL cells are green (best) or yellow (some performance-related cells may be allowed to be orange or red if absolutely necessary)</a:t>
+            <a:t>- settings are set acceptably when ALL value cells in Column C are green (best) or yellow (some performance-related cells may be allowed to be orange or red if absolutely necessary)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2022,19 +2022,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>- the execution commands at the top of the sheet should run the given case.  for large node counts and long runs it is recommended that the commands be submitted as a batch script instead of running interactively, to avoid wasting allocation</a:t>
+            <a:t>- the execution commands at the top of the sheet should run the given case, for one phase and one stage only.  for large node counts and long runs it is recommended that the commands be submitted as a batch script instead of running interactively, to avoid wasting allocation</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>- the number in the "performance fraction estimate" box should be inferred from a run.  The max tensor core rate on a large case for this code is ~ 82 TF.  so for example an ops_rate/proc of 1.64e+12 would be 2% efficiency.</a:t>
+            <a:t>- the number in the "performance fraction estimate" box should be inferred from a run.  The max tensor core rate on a large case for this code is ~ 82 TF.  so for example an ops_rate/proc of 1.64e+12 as reported from a run would be 2% efficiency.</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0"/>
-            <a:t>- NOTE: I/O time is not counted here - it could be inferred from an actual run on real data</a:t>
+            <a:t>- NOTE: I/O time is not counted here - it could be inferred from a run on real data</a:t>
           </a:r>
         </a:p>
         <a:p>

</xml_diff>

<commit_message>
Updates to settings tool.
</commit_message>
<xml_diff>
--- a/tools/CoMet_Settings_Tool.xlsx
+++ b/tools/CoMet_Settings_Tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjd/Desktop/DESKTOP_FILES/Genomics/genomics_gpu/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB75DAB-0F89-3F4C-A1E1-2840DCE9865B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E60A91A-25DF-FF46-A0EF-8883D4827466}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="660" windowWidth="26520" windowHeight="26480" xr2:uid="{FA80413B-B473-9946-BFAA-BCC79B485766}"/>
+    <workbookView xWindow="7520" yWindow="860" windowWidth="26520" windowHeight="26480" xr2:uid="{FA80413B-B473-9946-BFAA-BCC79B485766}"/>
   </bookViews>
   <sheets>
     <sheet name="CoMet_Settings_Tool" sheetId="6" r:id="rId1"/>
@@ -319,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{ED506729-3795-C745-95AB-0AEAC70FE358}">
+    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{65BAFC92-672F-6E45-82C0-2EBEB14BC698}">
       <text>
         <r>
           <rPr>
@@ -328,11 +328,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>tensor cores only available on some systems</t>
+          <t>for example, if this value is 10%, then require that the reported value by CoMet for a metric result must differ from the actual value that would be calculated in exact precision by no more than 10%</t>
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{56367034-E0EA-7C42-B15B-785625633B1D}">
+    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{6D6FC77A-85D2-6547-AD55-B344261C062E}">
       <text>
         <r>
           <rPr>
@@ -341,11 +341,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>limited by number of blocks in block row or slab</t>
+          <t>Current code limitation, may be improvable</t>
         </r>
       </text>
     </comment>
-    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{89A09225-5646-6F4C-B5A8-57724FF1992C}">
+    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{ED506729-3795-C745-95AB-0AEAC70FE358}">
       <text>
         <r>
           <rPr>
@@ -354,11 +354,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>can be &gt; 1 only if 3-way</t>
+          <t>tensor cores only available on some systems</t>
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{A43A2A89-B6CA-B341-97F3-A65248710DFD}">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{56367034-E0EA-7C42-B15B-785625633B1D}">
       <text>
         <r>
           <rPr>
@@ -367,11 +367,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>this should be only slightly less than a whole number, for good load balance - see next cell</t>
+          <t>limited by number of blocks in block row or slab</t>
         </r>
       </text>
     </comment>
-    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{F54BBA61-C6E4-B947-8FC4-DEAA11666DA4}">
+    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{89A09225-5646-6F4C-B5A8-57724FF1992C}">
       <text>
         <r>
           <rPr>
@@ -380,11 +380,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>similar to gpu pipeline len 3-way below</t>
+          <t>can be &gt; 1 only if 3-way</t>
         </r>
       </text>
     </comment>
-    <comment ref="C39" authorId="0" shapeId="0" xr:uid="{A7C87AB7-9A8A-C847-B94A-628E7D078BA2}">
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{A43A2A89-B6CA-B341-97F3-A65248710DFD}">
       <text>
         <r>
           <rPr>
@@ -393,11 +393,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>available memory limit on GPU may be ragged, may need to leave headroom</t>
+          <t>this should be only slightly less than a whole number, for good load balance - see next cell</t>
         </r>
       </text>
     </comment>
-    <comment ref="C40" authorId="0" shapeId="0" xr:uid="{ED64E219-E63C-D942-B4BB-BB76CB8D08C0}">
+    <comment ref="C39" authorId="0" shapeId="0" xr:uid="{F54BBA61-C6E4-B947-8FC4-DEAA11666DA4}">
       <text>
         <r>
           <rPr>
@@ -406,11 +406,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>percent used of available</t>
+          <t>similar to gpu pipeline len 3-way below</t>
         </r>
       </text>
     </comment>
-    <comment ref="C41" authorId="0" shapeId="0" xr:uid="{5EE7F4FA-CEB5-EC4B-98C6-CB339FD6A81D}">
+    <comment ref="C44" authorId="0" shapeId="0" xr:uid="{A7C87AB7-9A8A-C847-B94A-628E7D078BA2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>available memory limit on GPU may be ragged, may need to leave headroom</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{ED64E219-E63C-D942-B4BB-BB76CB8D08C0}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>percent used of available</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{5EE7F4FA-CEB5-EC4B-98C6-CB339FD6A81D}">
       <text>
         <r>
           <rPr>
@@ -424,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{3F0B7F9F-DFE6-114E-BF98-67DAAAC276D7}">
+    <comment ref="C50" authorId="0" shapeId="0" xr:uid="{3F0B7F9F-DFE6-114E-BF98-67DAAAC276D7}">
       <text>
         <r>
           <rPr>
@@ -437,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{0E6E5FB0-AA0A-2640-9C05-2B98230D3DA5}">
+    <comment ref="C51" authorId="0" shapeId="0" xr:uid="{0E6E5FB0-AA0A-2640-9C05-2B98230D3DA5}">
       <text>
         <r>
           <rPr>
@@ -450,7 +476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C49" authorId="0" shapeId="0" xr:uid="{9D68014A-D00F-394E-9808-8B8C39D5F02B}">
+    <comment ref="C54" authorId="0" shapeId="0" xr:uid="{9D68014A-D00F-394E-9808-8B8C39D5F02B}">
       <text>
         <r>
           <rPr>
@@ -463,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C56" authorId="0" shapeId="0" xr:uid="{2C1B4B88-7981-A74A-89A9-A7037DBB6656}">
+    <comment ref="C61" authorId="0" shapeId="0" xr:uid="{2C1B4B88-7981-A74A-89A9-A7037DBB6656}">
       <text>
         <r>
           <rPr>
@@ -476,7 +502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="0" shapeId="0" xr:uid="{44BC358F-FDD0-B942-85F1-218E53C613B3}">
+    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{44BC358F-FDD0-B942-85F1-218E53C613B3}">
       <text>
         <r>
           <rPr>
@@ -489,7 +515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C59" authorId="0" shapeId="0" xr:uid="{D3AB9A34-C0D1-C746-8520-94CAB011A1F0}">
+    <comment ref="C64" authorId="0" shapeId="0" xr:uid="{D3AB9A34-C0D1-C746-8520-94CAB011A1F0}">
       <text>
         <r>
           <rPr>
@@ -521,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C60" authorId="0" shapeId="0" xr:uid="{61D26C27-6EDA-FD48-A1F5-BCF57F6CFCE9}">
+    <comment ref="C65" authorId="0" shapeId="0" xr:uid="{61D26C27-6EDA-FD48-A1F5-BCF57F6CFCE9}">
       <text>
         <r>
           <rPr>
@@ -553,7 +579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C61" authorId="0" shapeId="0" xr:uid="{C19F36C0-780B-D34F-AFC0-17B17002334F}">
+    <comment ref="C66" authorId="0" shapeId="0" xr:uid="{C19F36C0-780B-D34F-AFC0-17B17002334F}">
       <text>
         <r>
           <rPr>
@@ -585,7 +611,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{2487F8E9-BE74-134D-92A4-3FC5FC35E35B}">
+    <comment ref="C68" authorId="0" shapeId="0" xr:uid="{2487F8E9-BE74-134D-92A4-3FC5FC35E35B}">
       <text>
         <r>
           <rPr>
@@ -598,7 +624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C64" authorId="0" shapeId="0" xr:uid="{10F1ADAC-D64A-CE40-A638-5C30C7DEBDD4}">
+    <comment ref="C69" authorId="0" shapeId="0" xr:uid="{10F1ADAC-D64A-CE40-A638-5C30C7DEBDD4}">
       <text>
         <r>
           <rPr>
@@ -611,7 +637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C65" authorId="0" shapeId="0" xr:uid="{76F522D1-1B6E-3A4B-BD9E-61519BE2A480}">
+    <comment ref="C70" authorId="0" shapeId="0" xr:uid="{76F522D1-1B6E-3A4B-BD9E-61519BE2A480}">
       <text>
         <r>
           <rPr>
@@ -624,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C68" authorId="0" shapeId="0" xr:uid="{D7956CF0-C904-DD44-8481-38B4D6DE3083}">
+    <comment ref="C73" authorId="0" shapeId="0" xr:uid="{D7956CF0-C904-DD44-8481-38B4D6DE3083}">
       <text>
         <r>
           <rPr>
@@ -642,7 +668,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="142">
   <si>
     <t>QUANTITY</t>
   </si>
@@ -981,9 +1007,6 @@
     <t>avg blocks/phase/proc</t>
   </si>
   <si>
-    <t xml:space="preserve">   . . . percent</t>
-  </si>
-  <si>
     <t xml:space="preserve">   . . . performance penalty</t>
   </si>
   <si>
@@ -1053,16 +1076,38 @@
   <si>
     <t>problem
 definition</t>
+  </si>
+  <si>
+    <t>num_field limit</t>
+  </si>
+  <si>
+    <t>GM_TALLY1_MAX_VALUE_BITS</t>
+  </si>
+  <si>
+    <t>. . . power 2</t>
+  </si>
+  <si>
+    <t>machine epsilon</t>
+  </si>
+  <si>
+    <t>required relative error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   . . . ratio (percent)</t>
+  </si>
+  <si>
+    <t>estimated relative error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1118,7 +1163,7 @@
       <name val="Calibri (Body)_x0000_"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1134,6 +1179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00F5FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFE00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1664,7 +1715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1912,6 +1963,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1940,6 +1994,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1951,8 +2011,8 @@
   <colors>
     <mruColors>
       <color rgb="FFFFFE00"/>
+      <color rgb="FFFF7F82"/>
       <color rgb="FF00FF01"/>
-      <color rgb="FFFF7F82"/>
       <color rgb="FF00F5FF"/>
     </mruColors>
   </colors>
@@ -2429,7 +2489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87649693-509E-D84D-8D62-271E15A24091}">
-  <dimension ref="A1:AC83"/>
+  <dimension ref="A1:AC88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -2448,8 +2508,8 @@
     <col min="11" max="11" width="15.83203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="10.83203125" style="2"/>
     <col min="13" max="13" width="1.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" style="53" customWidth="1"/>
-    <col min="15" max="15" width="11.1640625" style="53" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.5" style="53" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="53" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -2460,10 +2520,10 @@
     <row r="2" spans="1:29">
       <c r="A2" s="10"/>
       <c r="B2" s="62" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D2" s="64"/>
       <c r="E2" s="65"/>
@@ -2493,11 +2553,11 @@
       <c r="AC2" s="65"/>
     </row>
     <row r="3" spans="1:29">
-      <c r="A3" s="83" t="s">
-        <v>127</v>
+      <c r="A3" s="84" t="s">
+        <v>126</v>
       </c>
       <c r="B3" s="68" t="str">
-        <f>IF(C$16=L$16,CONCATENATE("bsub -P ",C2," -nnodes ",C50," -W 10 -Is $SHELL"),"")</f>
+        <f>IF(C$16=L$16,CONCATENATE("bsub -P ",C2," -nnodes ",C55," -W 10 -Is $SHELL"),"")</f>
         <v>bsub -P stf006 -nnodes 1334 -W 10 -Is $SHELL</v>
       </c>
       <c r="C3" s="69"/>
@@ -2529,21 +2589,21 @@
       <c r="AC3" s="70"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="84"/>
+      <c r="A4" s="85"/>
       <c r="B4" s="73" t="str">
         <f>IF(C$16=L$16,"executable=install_single_release_summit/bin/genomics_metric ar_opts='PAMI_IBV_ENABLE_DCT=1 PAMI_ENABLE_STRIPING=1 PAMI_IBV_ADAPTER_AFFINITY=0 PAMI_IBV_QP_SERVICE_LEVEL=8 PAMI_IBV_ENABLE_OOO_AR=1'","")</f>
         <v>executable=install_single_release_summit/bin/genomics_metric ar_opts='PAMI_IBV_ENABLE_DCT=1 PAMI_ENABLE_STRIPING=1 PAMI_IBV_ADAPTER_AFFINITY=0 PAMI_IBV_QP_SERVICE_LEVEL=8 PAMI_IBV_ENABLE_OOO_AR=1'</v>
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="84"/>
+      <c r="A5" s="85"/>
       <c r="B5" s="73" t="str">
-        <f>IF(C$16=L$16,CONCATENATE("launch_command=""env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs ",C49," --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"""),"")</f>
+        <f>IF(C$16=L$16,CONCATENATE("launch_command=""env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs ",C54," --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"""),"")</f>
         <v>launch_command="env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs 8004 --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"</v>
       </c>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="85"/>
+      <c r="A6" s="86"/>
       <c r="B6" s="74" t="str">
         <f>IF(C$16=L$16,CONCATENATE("$launch_command $executable --num_way ",C10," --metric_type ",C11," --sparse ",C12," --num_vector ",C13," --num_field ",C14," --all2all yes --compute_method GPU --num_proc_vector ",C19," --num_proc_field ",C20," --num_proc_repl ",C21," --tc ",O39," --num_tc_steps ",C23," --num_phase ",C24," --num_stage ",C25," --verbosity 1 --checksum no --phase_min ",MAX(0,C24-1)," --phase_max ",C24-1," --stage_min ",MAX(0,C25-1)," --stage_max ",C25-1),"")</f>
         <v>$launch_command $executable --num_way 3 --metric_type ccc --sparse yes --num_vector 1000000 --num_field 2000 --all2all yes --compute_method GPU --num_proc_vector 100 --num_proc_field 1 --num_proc_repl 80 --tc 1 --num_tc_steps 1 --num_phase 130 --num_stage 280 --verbosity 1 --checksum no --phase_min 129 --phase_max 129 --stage_min 279 --stage_max 279</v>
@@ -2615,11 +2675,11 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="86" t="s">
+      <c r="F8" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="87"/>
-      <c r="H8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="89"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="9" t="s">
@@ -2657,14 +2717,14 @@
       <c r="N9" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="O9" s="53">
+      <c r="O9" s="56">
         <f>1024*1024*1024</f>
         <v>1073741824</v>
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="89" t="s">
-        <v>135</v>
+      <c r="A10" s="90" t="s">
+        <v>134</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>6</v>
@@ -2696,13 +2756,13 @@
       <c r="N10" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="53">
+      <c r="O10" s="56">
         <f>1000000000</f>
         <v>1000000000</v>
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="90"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="32" t="s">
         <v>2</v>
       </c>
@@ -2858,7 +2918,7 @@
       </c>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="89" t="s">
+      <c r="A16" s="90" t="s">
         <v>108</v>
       </c>
       <c r="B16" s="31" t="s">
@@ -2900,7 +2960,7 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="90"/>
+      <c r="A17" s="91"/>
       <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
@@ -2965,7 +3025,7 @@
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="3">
         <f>100000000/30</f>
@@ -3185,8 +3245,8 @@
       </c>
     </row>
     <row r="26" spans="1:15">
-      <c r="B26" s="13"/>
-      <c r="C26" s="37"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="41"/>
       <c r="E26" s="4" t="s">
         <v>99</v>
       </c>
@@ -3214,13 +3274,14 @@
       </c>
     </row>
     <row r="27" spans="1:15">
-      <c r="B27" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="2">
-        <f>IF(C16=L15,0,O40)</f>
-        <v>2</v>
-      </c>
+      <c r="A27" s="10"/>
+      <c r="B27" s="95" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="94">
+        <v>0.1</v>
+      </c>
+      <c r="D27" s="29"/>
       <c r="E27" s="4" t="s">
         <v>100</v>
       </c>
@@ -3240,16 +3301,16 @@
       <c r="L27" s="53"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="B28" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="45">
-        <f>IF(O36=1,1+FLOOR(C19,2)/2,(C19+1)*(C19+2)/2)</f>
-        <v>5151</v>
+      <c r="B28" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="81">
+        <f>O55*10*C14</f>
+        <v>1.1919999999999999E-3</v>
       </c>
       <c r="L28" s="54"/>
       <c r="N28" s="53" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O28" s="53">
         <f>IF(C11=L11,O16,IF(O35=1,O22,2*O15))</f>
@@ -3258,15 +3319,15 @@
     </row>
     <row r="29" spans="1:15">
       <c r="B29" s="2" t="s">
-        <v>112</v>
+        <v>140</v>
       </c>
       <c r="C29" s="42">
-        <f>C24/C28</f>
-        <v>2.5237817899437003E-2</v>
+        <f>C28/C27</f>
+        <v>1.1919999999999998E-2</v>
       </c>
       <c r="L29" s="53"/>
       <c r="N29" s="53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O29" s="53">
         <f>IF(C11=L11,O16,IF(O35=1,4,2*O15))</f>
@@ -3274,22 +3335,22 @@
       </c>
     </row>
     <row r="30" spans="1:15">
-      <c r="B30" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="44">
-        <f>IF(O36=1,1,O42)</f>
-        <v>1E+30</v>
+      <c r="B30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="3">
+        <f>CEILING(O53,POWER(2,O38))/POWER(2,O38)-1</f>
+        <v>8388607</v>
       </c>
       <c r="L30" s="53"/>
     </row>
     <row r="31" spans="1:15">
       <c r="B31" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="42">
-        <f>C25/C30</f>
-        <v>2.7999999999999998E-28</v>
+        <v>140</v>
+      </c>
+      <c r="C31" s="83">
+        <f>C14/C30</f>
+        <v>2.3841860752327532E-4</v>
       </c>
       <c r="L31" s="53"/>
       <c r="N31" s="53" t="s">
@@ -3302,11 +3363,11 @@
     </row>
     <row r="32" spans="1:15">
       <c r="B32" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" s="61">
-        <f>IF(O36=1,(1+FLOOR(C19,2)/2)/C21/C24,(C19+1)*(C19+2)/C21/C24)</f>
-        <v>0.99057692307692313</v>
+        <v>109</v>
+      </c>
+      <c r="C32" s="2">
+        <f>IF(C16=L15,0,O40)</f>
+        <v>2</v>
       </c>
       <c r="L32" s="53"/>
       <c r="N32" s="53" t="s">
@@ -3318,12 +3379,12 @@
       </c>
     </row>
     <row r="33" spans="2:15">
-      <c r="B33" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="42">
-        <f>(CEILING(C32,1)-C32)/C32</f>
-        <v>9.5127159774800445E-3</v>
+      <c r="B33" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="45">
+        <f>IF(O36=1,1+FLOOR(C19,2)/2,(C19+1)*(C19+2)/2)</f>
+        <v>5151</v>
       </c>
       <c r="L33" s="53"/>
       <c r="N33" s="53" t="s">
@@ -3336,11 +3397,11 @@
     </row>
     <row r="34" spans="2:15">
       <c r="B34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="61">
-        <f>IF(O37=1,C72/6/C25,"N/A")</f>
-        <v>5.9571428571428573</v>
+        <v>140</v>
+      </c>
+      <c r="C34" s="42">
+        <f>C24/C33</f>
+        <v>2.5237817899437003E-2</v>
       </c>
       <c r="L34" s="53"/>
       <c r="N34" s="53" t="s">
@@ -3352,6 +3413,13 @@
       </c>
     </row>
     <row r="35" spans="2:15">
+      <c r="B35" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="44">
+        <f>IF(O36=1,1,O42)</f>
+        <v>1E+30</v>
+      </c>
       <c r="L35" s="53"/>
       <c r="N35" s="53" t="s">
         <v>84</v>
@@ -3363,11 +3431,11 @@
     </row>
     <row r="36" spans="2:15">
       <c r="B36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="3">
-        <f>O35*2*(CEILING(C73,C23)/C23)*(2*C71)*O22</f>
-        <v>160032000</v>
+        <v>140</v>
+      </c>
+      <c r="C36" s="42">
+        <f>C25/C35</f>
+        <v>2.7999999999999998E-28</v>
       </c>
       <c r="L36" s="53"/>
       <c r="N36" s="53" t="s">
@@ -3380,11 +3448,11 @@
     </row>
     <row r="37" spans="2:15">
       <c r="B37" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="3" t="str">
-        <f>IF(O36=1,3*C76+(2+O31)*C77+C36,"N/A")</f>
-        <v>N/A</v>
+        <v>111</v>
+      </c>
+      <c r="C37" s="61">
+        <f>IF(O36=1,(1+FLOOR(C19,2)/2)/C21/C24,(C19+1)*(C19+2)/C21/C24)</f>
+        <v>0.99057692307692313</v>
       </c>
       <c r="L37" s="53"/>
       <c r="N37" s="53" t="s">
@@ -3397,11 +3465,11 @@
     </row>
     <row r="38" spans="2:15">
       <c r="B38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="3">
-        <f>O37*((3*C76)+(2*C76+2*C77+O31*2*C77+O34*3*C77)+C36)</f>
-        <v>3386317128</v>
+        <v>112</v>
+      </c>
+      <c r="C38" s="42">
+        <f>(CEILING(C37,1)-C37)/C37</f>
+        <v>9.5127159774800445E-3</v>
       </c>
       <c r="L38" s="53"/>
       <c r="N38" s="53" t="s">
@@ -3414,11 +3482,11 @@
     </row>
     <row r="39" spans="2:15">
       <c r="B39" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="3">
-        <f>IF(O36=1,C37,C38)</f>
-        <v>3386317128</v>
+        <v>128</v>
+      </c>
+      <c r="C39" s="61">
+        <f>IF(O37=1,C77/6/C25,"N/A")</f>
+        <v>5.9571428571428573</v>
       </c>
       <c r="N39" s="53" t="s">
         <v>11</v>
@@ -3429,13 +3497,6 @@
       </c>
     </row>
     <row r="40" spans="2:15">
-      <c r="B40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="42">
-        <f>C39/I16</f>
-        <v>0.20748378856009558</v>
-      </c>
       <c r="N40" s="53" t="s">
         <v>110</v>
       </c>
@@ -3445,14 +3506,21 @@
     </row>
     <row r="41" spans="2:15">
       <c r="B41" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="42">
-        <f>C39/I16</f>
-        <v>0.20748378856009558</v>
+        <v>69</v>
+      </c>
+      <c r="C41" s="3">
+        <f>O35*2*(CEILING(C78,C23)/C23)*(2*C76)*O22</f>
+        <v>160032000</v>
       </c>
     </row>
     <row r="42" spans="2:15">
+      <c r="B42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="3" t="str">
+        <f>IF(O36=1,3*C81+(2+O31)*C82+C41,"N/A")</f>
+        <v>N/A</v>
+      </c>
       <c r="N42" s="53" t="s">
         <v>94</v>
       </c>
@@ -3462,20 +3530,20 @@
     </row>
     <row r="43" spans="2:15">
       <c r="B43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="3" t="str">
-        <f>IF(O36=1,C76+(C37-C36)+2*C80+C83,"N/A")</f>
-        <v>N/A</v>
+        <v>68</v>
+      </c>
+      <c r="C43" s="3">
+        <f>O37*((3*C81)+(2*C81+2*C82+O31*2*C82+O34*3*C82)+C41)</f>
+        <v>3386317128</v>
       </c>
     </row>
     <row r="44" spans="2:15">
       <c r="B44" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C44" s="3">
-        <f>IF(O37=1,C76+(C38-C36)+3*C80+C83,"N/A")</f>
-        <v>46448807904</v>
+        <f>IF(O36=1,C42,C43)</f>
+        <v>3386317128</v>
       </c>
       <c r="N44" s="53" t="s">
         <v>51</v>
@@ -3487,11 +3555,11 @@
     </row>
     <row r="45" spans="2:15">
       <c r="B45" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C45" s="3">
-        <f>IF(O36=1,C43,C44)</f>
-        <v>46448807904</v>
+        <v>79</v>
+      </c>
+      <c r="C45" s="42">
+        <f>C44/I16</f>
+        <v>0.20748378856009558</v>
       </c>
       <c r="N45" s="53" t="s">
         <v>52</v>
@@ -3503,11 +3571,11 @@
     </row>
     <row r="46" spans="2:15">
       <c r="B46" s="2" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="C46" s="42">
-        <f>C45/I17</f>
-        <v>0.61798319092818665</v>
+        <f>C44/I16</f>
+        <v>0.20748378856009558</v>
       </c>
       <c r="N46" s="53" t="s">
         <v>105</v>
@@ -3528,11 +3596,11 @@
     </row>
     <row r="48" spans="2:15">
       <c r="B48" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="3">
-        <f>C19*C20*C21</f>
-        <v>8000</v>
+        <v>71</v>
+      </c>
+      <c r="C48" s="3" t="str">
+        <f>IF(O36=1,C81+(C42-C41)+2*C85+C88,"N/A")</f>
+        <v>N/A</v>
       </c>
       <c r="N48" s="53" t="s">
         <v>55</v>
@@ -3544,11 +3612,11 @@
     </row>
     <row r="49" spans="2:15">
       <c r="B49" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" s="36">
-        <f>CEILING(C48,I11)</f>
-        <v>8004</v>
+        <v>72</v>
+      </c>
+      <c r="C49" s="3">
+        <f>IF(O37=1,C81+(C43-C41)+3*C85+C88,"N/A")</f>
+        <v>46448807904</v>
       </c>
       <c r="N49" s="53" t="s">
         <v>58</v>
@@ -3559,12 +3627,12 @@
       </c>
     </row>
     <row r="50" spans="2:15">
-      <c r="B50" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="C50" s="82">
-        <f>C49/I11</f>
-        <v>1334</v>
+      <c r="B50" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="3">
+        <f>IF(O36=1,C48,C49)</f>
+        <v>46448807904</v>
       </c>
       <c r="D50" s="29"/>
       <c r="N50" s="53" t="s">
@@ -3577,258 +3645,316 @@
     </row>
     <row r="51" spans="2:15">
       <c r="B51" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="81">
-        <f>C50/I13</f>
-        <v>0.28949652777777779</v>
+        <v>80</v>
+      </c>
+      <c r="C51" s="42">
+        <f>C50/I17</f>
+        <v>0.61798319092818665</v>
       </c>
     </row>
     <row r="52" spans="2:15">
-      <c r="B52" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="42">
-        <f>C51/0.2</f>
-        <v>1.4474826388888888</v>
+      <c r="N52" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="O52" s="53">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
+      <c r="B53" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C53" s="3">
+        <f>C19*C20*C21</f>
+        <v>8000</v>
+      </c>
+      <c r="N53" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="O53" s="56">
+        <f>POWER(2,O52)</f>
+        <v>67108864</v>
       </c>
     </row>
     <row r="54" spans="2:15">
       <c r="B54" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C54" s="3">
-        <f>IF(O35=1,CEILING(C73,C23)/C23,IF(O33=0,C73,CEILING(C73,64)/64))</f>
-        <v>2000</v>
+        <v>116</v>
+      </c>
+      <c r="C54" s="36">
+        <f>CEILING(C53,I11)</f>
+        <v>8004</v>
       </c>
     </row>
     <row r="55" spans="2:15">
-      <c r="B55" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="3">
-        <f>C71*(1+O35)</f>
-        <v>20004</v>
+      <c r="B55" s="79" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="82">
+        <f>C54/I11</f>
+        <v>1334</v>
+      </c>
+      <c r="N55" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="O55" s="53">
+        <f>IF(C17=L18,0.0000000596,0.000000000000000111)</f>
+        <v>5.9599999999999998E-8</v>
       </c>
     </row>
     <row r="56" spans="2:15">
       <c r="B56" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C56" s="43">
-        <f>MAX(C54/C55,C55/C54)</f>
-        <v>10.002000000000001</v>
+        <v>131</v>
+      </c>
+      <c r="C56" s="81">
+        <f>C55/I13</f>
+        <v>0.28949652777777779</v>
       </c>
     </row>
     <row r="57" spans="2:15">
       <c r="B57" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C57" s="3">
-        <f>2*C54*C55*O28+C55*C55*O29</f>
-        <v>1760672064</v>
+        <v>130</v>
+      </c>
+      <c r="C57" s="42">
+        <f>C56/0.2</f>
+        <v>1.4474826388888888</v>
       </c>
     </row>
     <row r="59" spans="2:15">
       <c r="B59" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C59" s="3">
+        <f>IF(O35=1,CEILING(C78,C23)/C23,IF(O33=0,C78,CEILING(C78,64)/64))</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="60" spans="2:15">
+      <c r="B60" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" s="3">
+        <f>C76*(1+O35)</f>
+        <v>20004</v>
+      </c>
+    </row>
+    <row r="61" spans="2:15">
+      <c r="B61" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="43">
+        <f>MAX(C59/C60,C60/C59)</f>
+        <v>10.002000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="B62" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" s="3">
+        <f>2*C59*C60*O28+C60*C60*O29</f>
+        <v>1760672064</v>
+      </c>
+    </row>
+    <row r="64" spans="2:15">
+      <c r="B64" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C59" s="3" t="str">
+      <c r="C64" s="3" t="str">
         <f>IF(O36=1,CEILING(CEILING(CEILING(C19+1,2)/2,C21)/C21,C24)/C24,"N/A")</f>
         <v>N/A</v>
       </c>
     </row>
-    <row r="60" spans="2:15">
-      <c r="B60" s="2" t="s">
+    <row r="65" spans="1:7">
+      <c r="B65" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C65" s="3">
         <f>IF(O37=1,CEILING((C19+1)*(C19+2),C21*C24)/(C21*C24),"N/A")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="2:15">
-      <c r="B61" s="2" t="s">
+    <row r="66" spans="1:7">
+      <c r="B66" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="3">
-        <f>IF(O37=1,C78,"N/A")</f>
+      <c r="C66" s="3">
+        <f>IF(O37=1,C83,"N/A")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="2:15">
-      <c r="B63" s="2" t="s">
+    <row r="67" spans="1:7">
+      <c r="D67" s="29"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="B68" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C63" s="46">
+      <c r="C68" s="46">
         <f>IF(O36=1,C14*C13*C13/2,C14*C13*C13*C13/6)</f>
         <v>3.3333333333333331E+20</v>
       </c>
     </row>
-    <row r="64" spans="2:15">
-      <c r="B64" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C64" s="58">
+    <row r="69" spans="1:7">
+      <c r="B69" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="58">
         <f>I21*1000000000000000</f>
         <v>8.1611E+16</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
-      <c r="B65" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" s="59">
+    <row r="70" spans="1:7">
+      <c r="B70" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="59">
         <f>1.75/82</f>
         <v>2.1341463414634148E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
-      <c r="B66" s="13" t="s">
+    <row r="71" spans="1:7">
+      <c r="A71" s="92" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" s="80">
+        <f>C69*C70</f>
+        <v>1741698170731707.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="93"/>
+      <c r="B72" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="80">
-        <f>C64*C65</f>
-        <v>1741698170731707.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="B67" s="79" t="s">
-        <v>123</v>
-      </c>
-      <c r="C67" s="82">
-        <f>C63/C66/3600*I13</f>
+      <c r="C72" s="82">
+        <f>C68/C71/3600*I13</f>
         <v>244971.6453956078</v>
-      </c>
-      <c r="D67" s="29"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="B68" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C68" s="81">
-        <f>C67/I19</f>
-        <v>0.81657215131869265</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="C69" s="1"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="91" t="s">
-        <v>133</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C71" s="3">
-        <f>CEILING(CEILING(C13,C19)/C19,IF(O37=1,6,1))</f>
-        <v>10002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="92"/>
-      <c r="B72" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C72" s="3">
-        <f>IF(AND(O35=0,O37=0),C71,IF(O35=0,CEILING(C71,6),IF(O37=0,CEILING(C71,4),CEILING(C71,24))))</f>
-        <v>10008</v>
       </c>
       <c r="E72" s="51"/>
     </row>
     <row r="73" spans="1:7">
       <c r="B73" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C73" s="3">
-        <f>CEILING(C14,C20)/C20</f>
-        <v>2000</v>
+        <v>124</v>
+      </c>
+      <c r="C73" s="81">
+        <f>C72/I19</f>
+        <v>0.81657215131869265</v>
       </c>
     </row>
     <row r="74" spans="1:7">
+      <c r="C74" s="1"/>
       <c r="G74" s="52"/>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="B75" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C75" s="3">
-        <f>CEILING(C73*O44,O12)/O12</f>
-        <v>500</v>
-      </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="10"/>
       <c r="B76" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C76" s="3">
-        <f>C75*C71</f>
-        <v>5001000</v>
+        <f>CEILING(CEILING(C13,C19)/C19,IF(O37=1,6,1))</f>
+        <v>10002</v>
       </c>
       <c r="D76" s="29"/>
     </row>
     <row r="77" spans="1:7">
       <c r="B77" s="2" t="s">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="C77" s="3">
-        <f>O46*C71*C71</f>
-        <v>1600640064</v>
+        <f>IF(AND(O35=0,O37=0),C76,IF(O35=0,CEILING(C76,6),IF(O37=0,CEILING(C76,4),CEILING(C76,24))))</f>
+        <v>10008</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="B78" s="2" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="C78" s="3">
-        <f>CEILING(C71,6*C25)/(6*C25)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="B79" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C79" s="3">
-        <f>O50*C71*C71*C78</f>
-        <v>43217281728</v>
+        <f>CEILING(C14,C20)/C20</f>
+        <v>2000</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="B80" s="2" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C80" s="3">
-        <f>C71*O16*IF(O36=1,1,(1+O31)*(1+O32))</f>
-        <v>80016</v>
+        <f>CEILING(C78*O44,O12)/O12</f>
+        <v>500</v>
       </c>
     </row>
     <row r="81" spans="2:3">
       <c r="B81" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C81" s="3" t="str">
-        <f>IF(O36=1,C77*C59,"N/A")</f>
-        <v>N/A</v>
+        <v>63</v>
+      </c>
+      <c r="C81" s="3">
+        <f>C80*C76</f>
+        <v>5001000</v>
       </c>
     </row>
     <row r="82" spans="2:3">
       <c r="B82" s="2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C82" s="3">
-        <f>IF(O37=1,C79*C60,"N/A")</f>
-        <v>43217281728</v>
+        <f>O46*C76*C76</f>
+        <v>1600640064</v>
       </c>
     </row>
     <row r="83" spans="2:3">
       <c r="B83" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="3">
+        <f>CEILING(C76,6*C25)/(6*C25)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" s="3">
+        <f>O50*C76*C76*C83</f>
+        <v>43217281728</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="B85" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" s="3">
+        <f>C76*O16*IF(O36=1,1,(1+O31)*(1+O32))</f>
+        <v>80016</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C86" s="3" t="str">
+        <f>IF(O36=1,C82*C64,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="B87" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="3">
+        <f>IF(O37=1,C84*C65,"N/A")</f>
+        <v>43217281728</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C83" s="3">
-        <f>IF(O36=1,C81,C82)</f>
+      <c r="C88" s="3">
+        <f>IF(O36=1,C86,C87)</f>
         <v>43217281728</v>
       </c>
     </row>
@@ -3840,8 +3966,8 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A71:A72"/>
   </mergeCells>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="C44">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="$I$16 * 0.95"/>
@@ -3852,8 +3978,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="C55">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="$I$13 * 0.98"/>
@@ -3864,8 +3990,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="C50">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="$I$17 * 0.95"/>
@@ -3876,11 +4002,35 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C45">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.95"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFFFE00"/>
+        <color rgb="FFFF7F82"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0.95"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFFFE00"/>
+        <color rgb="FFFF7F82"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.95"/>
+        <cfvo type="num" val="0.98"/>
         <cfvo type="num" val="1"/>
         <color rgb="FF00FF01"/>
         <color rgb="FFFFFE00"/>
@@ -3892,30 +4042,6 @@
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.95"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FF00FF01"/>
-        <color rgb="FFFFFE00"/>
-        <color rgb="FFFF7F82"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0.98"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FF00FF01"/>
-        <color rgb="FFFFFE00"/>
-        <color rgb="FFFF7F82"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.7"/>
         <cfvo type="num" val="1"/>
         <color rgb="FFFF7F82"/>
@@ -3924,8 +4050,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="C38">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.2"/>
@@ -3936,38 +4062,38 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="C34">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="formula" val="IF($C$29&gt;1,0.1,$O$42)"/>
+        <cfvo type="formula" val="IF($C$34&gt;1,0.1,$O$42)"/>
         <color rgb="FF00FF01"/>
         <color rgb="FFFF7F82"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="colorScale" priority="15">
+  <conditionalFormatting sqref="C36">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
-        <cfvo type="formula" val="IF($C$25&gt;$C$30,0.1,$O$42)"/>
+        <cfvo type="formula" val="IF($C$25&gt;$C$35,0.1,$O$42)"/>
         <color rgb="FF00FF01"/>
         <color rgb="FFFF7F82"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="C32">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="-2"/>
-        <cfvo type="formula" val="IF($O$39&gt;$C$27,-1,$O$42)"/>
+        <cfvo type="formula" val="IF($O$39&gt;$C$32,-1,$O$42)"/>
         <color rgb="FF00FF01"/>
         <color rgb="FFFF7F82"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="C64">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -3978,8 +4104,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="C66">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="1"/>
         <cfvo type="num" val="5"/>
@@ -3990,8 +4116,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C73">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="2"/>
@@ -4002,13 +4128,33 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C57">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0.95"/>
         <cfvo type="num" val="1"/>
         <color rgb="FFFF7F82"/>
         <color rgb="FF00FF01"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFF7F82"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFF7F82"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated CoMet settings tool with prelim. Perlmutter info, new features.
</commit_message>
<xml_diff>
--- a/tools/CoMet_Settings_Tool.xlsx
+++ b/tools/CoMet_Settings_Tool.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjd/Desktop/DESKTOP_FILES/Genomics/genomics_gpu/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E60A91A-25DF-FF46-A0EF-8883D4827466}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD2E289-BA58-834C-85CB-DE550A2C77A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="860" windowWidth="26520" windowHeight="26480" xr2:uid="{FA80413B-B473-9946-BFAA-BCC79B485766}"/>
+    <workbookView xWindow="14640" yWindow="600" windowWidth="33640" windowHeight="30340" xr2:uid="{FA80413B-B473-9946-BFAA-BCC79B485766}"/>
   </bookViews>
   <sheets>
     <sheet name="CoMet_Settings_Tool" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -319,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{65BAFC92-672F-6E45-82C0-2EBEB14BC698}">
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{65BAFC92-672F-6E45-82C0-2EBEB14BC698}">
       <text>
         <r>
           <rPr>
@@ -332,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C30" authorId="0" shapeId="0" xr:uid="{6D6FC77A-85D2-6547-AD55-B344261C062E}">
+    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{6D6FC77A-85D2-6547-AD55-B344261C062E}">
       <text>
         <r>
           <rPr>
@@ -345,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C32" authorId="0" shapeId="0" xr:uid="{ED506729-3795-C745-95AB-0AEAC70FE358}">
+    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{ED506729-3795-C745-95AB-0AEAC70FE358}">
       <text>
         <r>
           <rPr>
@@ -358,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C33" authorId="0" shapeId="0" xr:uid="{56367034-E0EA-7C42-B15B-785625633B1D}">
+    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{56367034-E0EA-7C42-B15B-785625633B1D}">
       <text>
         <r>
           <rPr>
@@ -371,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C35" authorId="0" shapeId="0" xr:uid="{89A09225-5646-6F4C-B5A8-57724FF1992C}">
+    <comment ref="C36" authorId="0" shapeId="0" xr:uid="{89A09225-5646-6F4C-B5A8-57724FF1992C}">
       <text>
         <r>
           <rPr>
@@ -384,7 +388,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{A43A2A89-B6CA-B341-97F3-A65248710DFD}">
+    <comment ref="C38" authorId="0" shapeId="0" xr:uid="{A43A2A89-B6CA-B341-97F3-A65248710DFD}">
       <text>
         <r>
           <rPr>
@@ -397,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C39" authorId="0" shapeId="0" xr:uid="{F54BBA61-C6E4-B947-8FC4-DEAA11666DA4}">
+    <comment ref="C40" authorId="0" shapeId="0" xr:uid="{F54BBA61-C6E4-B947-8FC4-DEAA11666DA4}">
       <text>
         <r>
           <rPr>
@@ -410,7 +414,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C44" authorId="0" shapeId="0" xr:uid="{A7C87AB7-9A8A-C847-B94A-628E7D078BA2}">
+    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{A7C87AB7-9A8A-C847-B94A-628E7D078BA2}">
       <text>
         <r>
           <rPr>
@@ -423,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C45" authorId="0" shapeId="0" xr:uid="{ED64E219-E63C-D942-B4BB-BB76CB8D08C0}">
+    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{ED64E219-E63C-D942-B4BB-BB76CB8D08C0}">
       <text>
         <r>
           <rPr>
@@ -436,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{5EE7F4FA-CEB5-EC4B-98C6-CB339FD6A81D}">
+    <comment ref="C47" authorId="0" shapeId="0" xr:uid="{5EE7F4FA-CEB5-EC4B-98C6-CB339FD6A81D}">
       <text>
         <r>
           <rPr>
@@ -450,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C50" authorId="0" shapeId="0" xr:uid="{3F0B7F9F-DFE6-114E-BF98-67DAAAC276D7}">
+    <comment ref="C51" authorId="0" shapeId="0" xr:uid="{3F0B7F9F-DFE6-114E-BF98-67DAAAC276D7}">
       <text>
         <r>
           <rPr>
@@ -463,7 +467,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C51" authorId="0" shapeId="0" xr:uid="{0E6E5FB0-AA0A-2640-9C05-2B98230D3DA5}">
+    <comment ref="C52" authorId="0" shapeId="0" xr:uid="{0E6E5FB0-AA0A-2640-9C05-2B98230D3DA5}">
       <text>
         <r>
           <rPr>
@@ -476,7 +480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C54" authorId="0" shapeId="0" xr:uid="{9D68014A-D00F-394E-9808-8B8C39D5F02B}">
+    <comment ref="C55" authorId="0" shapeId="0" xr:uid="{9D68014A-D00F-394E-9808-8B8C39D5F02B}">
       <text>
         <r>
           <rPr>
@@ -489,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C61" authorId="0" shapeId="0" xr:uid="{2C1B4B88-7981-A74A-89A9-A7037DBB6656}">
+    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{2C1B4B88-7981-A74A-89A9-A7037DBB6656}">
       <text>
         <r>
           <rPr>
@@ -502,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C62" authorId="0" shapeId="0" xr:uid="{44BC358F-FDD0-B942-85F1-218E53C613B3}">
+    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{44BC358F-FDD0-B942-85F1-218E53C613B3}">
       <text>
         <r>
           <rPr>
@@ -515,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C64" authorId="0" shapeId="0" xr:uid="{D3AB9A34-C0D1-C746-8520-94CAB011A1F0}">
+    <comment ref="C65" authorId="0" shapeId="0" xr:uid="{D3AB9A34-C0D1-C746-8520-94CAB011A1F0}">
       <text>
         <r>
           <rPr>
@@ -547,7 +551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C65" authorId="0" shapeId="0" xr:uid="{61D26C27-6EDA-FD48-A1F5-BCF57F6CFCE9}">
+    <comment ref="C66" authorId="0" shapeId="0" xr:uid="{61D26C27-6EDA-FD48-A1F5-BCF57F6CFCE9}">
       <text>
         <r>
           <rPr>
@@ -579,7 +583,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C66" authorId="0" shapeId="0" xr:uid="{C19F36C0-780B-D34F-AFC0-17B17002334F}">
+    <comment ref="C67" authorId="0" shapeId="0" xr:uid="{C19F36C0-780B-D34F-AFC0-17B17002334F}">
       <text>
         <r>
           <rPr>
@@ -611,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C68" authorId="0" shapeId="0" xr:uid="{2487F8E9-BE74-134D-92A4-3FC5FC35E35B}">
+    <comment ref="C69" authorId="0" shapeId="0" xr:uid="{2487F8E9-BE74-134D-92A4-3FC5FC35E35B}">
       <text>
         <r>
           <rPr>
@@ -624,7 +628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C69" authorId="0" shapeId="0" xr:uid="{10F1ADAC-D64A-CE40-A638-5C30C7DEBDD4}">
+    <comment ref="C70" authorId="0" shapeId="0" xr:uid="{10F1ADAC-D64A-CE40-A638-5C30C7DEBDD4}">
       <text>
         <r>
           <rPr>
@@ -637,7 +641,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C70" authorId="0" shapeId="0" xr:uid="{76F522D1-1B6E-3A4B-BD9E-61519BE2A480}">
+    <comment ref="C71" authorId="0" shapeId="0" xr:uid="{76F522D1-1B6E-3A4B-BD9E-61519BE2A480}">
       <text>
         <r>
           <rPr>
@@ -650,7 +654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C73" authorId="0" shapeId="0" xr:uid="{D7956CF0-C904-DD44-8481-38B4D6DE3083}">
+    <comment ref="C74" authorId="0" shapeId="0" xr:uid="{D7956CF0-C904-DD44-8481-38B4D6DE3083}">
       <text>
         <r>
           <rPr>
@@ -668,7 +672,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="175">
   <si>
     <t>QUANTITY</t>
   </si>
@@ -727,9 +731,6 @@
     <t>system</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>SYSTEM</t>
   </si>
   <si>
@@ -796,9 +797,6 @@
     <t>CPU mem per rank (bytes)</t>
   </si>
   <si>
-    <t>(other)</t>
-  </si>
-  <si>
     <t>num_proc_vector</t>
   </si>
   <si>
@@ -826,9 +824,6 @@
     <t>bits per vector elt</t>
   </si>
   <si>
-    <t>bytes per metric elt</t>
-  </si>
-  <si>
     <t>contstants etc.</t>
   </si>
   <si>
@@ -847,12 +842,6 @@
     <t>bytes per C</t>
   </si>
   <si>
-    <t>bytes per metric</t>
-  </si>
-  <si>
-    <t>bytes per elt index</t>
-  </si>
-  <si>
     <t>num vector local</t>
   </si>
   <si>
@@ -983,15 +972,6 @@
   </si>
   <si>
     <t>actual</t>
-  </si>
-  <si>
-    <t>bytes per metric elt 2-way</t>
-  </si>
-  <si>
-    <t>bytes / metrics 3d slice / stage</t>
-  </si>
-  <si>
-    <t>planes / 3d slice / stage</t>
   </si>
   <si>
     <t>solver
@@ -1097,6 +1077,129 @@
   </si>
   <si>
     <t>estimated relative error</t>
+  </si>
+  <si>
+    <t>Perlmutter</t>
+  </si>
+  <si>
+    <t>duo</t>
+  </si>
+  <si>
+    <t>5 (B1)</t>
+  </si>
+  <si>
+    <t>6 (INT4)</t>
+  </si>
+  <si>
+    <t>metrics_shrink</t>
+  </si>
+  <si>
+    <t>sizeof B1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        2-way duo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        3-way duo</t>
+  </si>
+  <si>
+    <t>is_duo</t>
+  </si>
+  <si>
+    <t>bytes per metric item</t>
+  </si>
+  <si>
+    <t>is_shrink -- FIX</t>
+  </si>
+  <si>
+    <t>ComputeMetrics3Way::compute_all2all_</t>
+  </si>
+  <si>
+    <t>Vectors</t>
+  </si>
+  <si>
+    <t>mirrored_buf vectors</t>
+  </si>
+  <si>
+    <t>mirrored_buf metrics</t>
+  </si>
+  <si>
+    <t>TOTAL CPU</t>
+  </si>
+  <si>
+    <t>TOTAL GPU</t>
+  </si>
+  <si>
+    <t>MEMORY:</t>
+  </si>
+  <si>
+    <t>ComputeMetrics3WayBlock::ComputeMetrics3WayBlock</t>
+  </si>
+  <si>
+    <t>CompressedBuf</t>
+  </si>
+  <si>
+    <t>form_matX_tc -- FIX</t>
+  </si>
+  <si>
+    <t>is_compress_enabled -- FIX</t>
+  </si>
+  <si>
+    <t>TCBufs::malloc</t>
+  </si>
+  <si>
+    <t>other CPU</t>
+  </si>
+  <si>
+    <t>other GPU</t>
+  </si>
+  <si>
+    <t>driver</t>
+  </si>
+  <si>
+    <t>GMMetrics_create</t>
+  </si>
+  <si>
+    <t>is_using_xor -- FIX</t>
+  </si>
+  <si>
+    <t>is_threshold_tc -- FIX</t>
+  </si>
+  <si>
+    <t>num_metrics_local</t>
+  </si>
+  <si>
+    <t>metric items per metric</t>
+  </si>
+  <si>
+    <t>bytes per metric (elt)</t>
+  </si>
+  <si>
+    <t>bytes per metric (elt) 2-way</t>
+  </si>
+  <si>
+    <t>bytes per metric index</t>
+  </si>
+  <si>
+    <t>bytes per metric (elt) + extras</t>
+  </si>
+  <si>
+    <t>num_metrics_local 2-way</t>
+  </si>
+  <si>
+    <t>num_metrics_local 3-way</t>
+  </si>
+  <si>
+    <t>planes / 3d slice / stage / phase</t>
+  </si>
+  <si>
+    <t>bytes / metrics 3d slice / stage / phase</t>
+  </si>
+  <si>
+    <t>bytes for metrics + indexing</t>
+  </si>
+  <si>
+    <t>ComputeMetrics2Way::ComputeMetrics2Way</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1212,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1162,6 +1265,12 @@
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1189,7 +1298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1711,11 +1820,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1876,9 +2011,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1966,6 +2098,40 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1990,16 +2156,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2032,15 +2195,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:colOff>279401</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>112060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>854636</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>99360</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2055,8 +2218,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6654800" y="5740400"/>
-          <a:ext cx="5981700" cy="7302500"/>
+          <a:off x="7152342" y="7433236"/>
+          <a:ext cx="6521823" cy="7517653"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2184,12 +2347,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Wayne Joubert" id="{4FDEEA99-810F-2C4C-BD96-7D4A3D6E0D28}" userId="Wayne Joubert" providerId="None"/>
-</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2489,152 +2646,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87649693-509E-D84D-8D62-271E15A24091}">
-  <dimension ref="A1:AC88"/>
+  <dimension ref="A1:AC112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="1.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
     <col min="10" max="10" width="1.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="15" style="2" customWidth="1"/>
     <col min="13" max="13" width="1.83203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="27.5" style="53" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" style="53" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="14.1640625" style="53" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="5.1640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="3" style="1" customWidth="1"/>
+    <col min="19" max="19" width="41" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
       <c r="B1" s="30"/>
       <c r="C1" s="36"/>
+      <c r="Q1" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="10"/>
-      <c r="B2" s="62" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
+      <c r="B2" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64"/>
       <c r="F2" s="30"/>
-      <c r="G2" s="65"/>
+      <c r="G2" s="64"/>
       <c r="H2" s="30"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="65"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
-      <c r="AC2" s="65"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="30">
+        <f>Q1+1</f>
+        <v>2</v>
+      </c>
+      <c r="R2" s="64"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="64"/>
+      <c r="V2" s="64"/>
+      <c r="W2" s="64"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
     </row>
     <row r="3" spans="1:29">
-      <c r="A3" s="84" t="s">
-        <v>126</v>
-      </c>
-      <c r="B3" s="68" t="str">
-        <f>IF(C$16=L$16,CONCATENATE("bsub -P ",C2," -nnodes ",C55," -W 10 -Is $SHELL"),"")</f>
-        <v>bsub -P stf006 -nnodes 1334 -W 10 -Is $SHELL</v>
-      </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
+      <c r="A3" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="67" t="str">
+        <f>IF(C$16=L$20,CONCATENATE("bsub -P ",C2," -nnodes ",C56," -W 10 -Is $SHELL"),"")</f>
+        <v/>
+      </c>
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="30">
+        <f t="shared" ref="Q3:Q66" si="0">Q2+1</f>
+        <v>3</v>
+      </c>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="69"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="69"/>
+      <c r="AB3" s="69"/>
+      <c r="AC3" s="69"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="85"/>
-      <c r="B4" s="73" t="str">
-        <f>IF(C$16=L$16,"executable=install_single_release_summit/bin/genomics_metric ar_opts='PAMI_IBV_ENABLE_DCT=1 PAMI_ENABLE_STRIPING=1 PAMI_IBV_ADAPTER_AFFINITY=0 PAMI_IBV_QP_SERVICE_LEVEL=8 PAMI_IBV_ENABLE_OOO_AR=1'","")</f>
-        <v>executable=install_single_release_summit/bin/genomics_metric ar_opts='PAMI_IBV_ENABLE_DCT=1 PAMI_ENABLE_STRIPING=1 PAMI_IBV_ADAPTER_AFFINITY=0 PAMI_IBV_QP_SERVICE_LEVEL=8 PAMI_IBV_ENABLE_OOO_AR=1'</v>
+      <c r="A4" s="96"/>
+      <c r="B4" s="72" t="str">
+        <f>IF(C$16=L$20,"executable=install_single_release_summit/bin/genomics_metric ar_opts='PAMI_IBV_ENABLE_DCT=1 PAMI_ENABLE_STRIPING=1 PAMI_IBV_ADAPTER_AFFINITY=0 PAMI_IBV_QP_SERVICE_LEVEL=8 PAMI_IBV_ENABLE_OOO_AR=1'","")</f>
+        <v/>
+      </c>
+      <c r="Q4" s="30">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="85"/>
-      <c r="B5" s="73" t="str">
-        <f>IF(C$16=L$16,CONCATENATE("launch_command=""env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs ",C54," --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"""),"")</f>
-        <v>launch_command="env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs 8004 --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"</v>
+      <c r="A5" s="96"/>
+      <c r="B5" s="72" t="str">
+        <f>IF(C$16=L$20,CONCATENATE("launch_command=""env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs ",C55," --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"""),"")</f>
+        <v/>
+      </c>
+      <c r="Q5" s="30">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="86"/>
-      <c r="B6" s="74" t="str">
-        <f>IF(C$16=L$16,CONCATENATE("$launch_command $executable --num_way ",C10," --metric_type ",C11," --sparse ",C12," --num_vector ",C13," --num_field ",C14," --all2all yes --compute_method GPU --num_proc_vector ",C19," --num_proc_field ",C20," --num_proc_repl ",C21," --tc ",O39," --num_tc_steps ",C23," --num_phase ",C24," --num_stage ",C25," --verbosity 1 --checksum no --phase_min ",MAX(0,C24-1)," --phase_max ",C24-1," --stage_min ",MAX(0,C25-1)," --stage_max ",C25-1),"")</f>
-        <v>$launch_command $executable --num_way 3 --metric_type ccc --sparse yes --num_vector 1000000 --num_field 2000 --all2all yes --compute_method GPU --num_proc_vector 100 --num_proc_field 1 --num_proc_repl 80 --tc 1 --num_tc_steps 1 --num_phase 130 --num_stage 280 --verbosity 1 --checksum no --phase_min 129 --phase_max 129 --stage_min 279 --stage_max 279</v>
-      </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="77"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="77"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="78"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="76"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="76"/>
-      <c r="U6" s="76"/>
-      <c r="V6" s="76"/>
-      <c r="W6" s="76"/>
-      <c r="X6" s="76"/>
-      <c r="Y6" s="76"/>
-      <c r="Z6" s="76"/>
-      <c r="AA6" s="76"/>
-      <c r="AB6" s="76"/>
-      <c r="AC6" s="76"/>
+      <c r="A6" s="97"/>
+      <c r="B6" s="73" t="str">
+        <f>IF(C$16=L$20,CONCATENATE("$launch_command $executable --num_way ",C10," --metric_type ",C11," --sparse ",C12," --num_vector ",C13," --num_field ",C14," --all2all yes --compute_method GPU --num_proc_vector ",C19," --num_proc_field ",C20," --num_proc_repl ",C21," --tc ",O41," --num_tc_steps ",C23," --num_phase ",C24," --num_stage ",C25," --verbosity 1 --checksum no --phase_min ",MAX(0,C24-1)," --phase_max ",C24-1," --stage_min ",MAX(0,C25-1)," --stage_max ",C25-1),"")</f>
+        <v/>
+      </c>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="77"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="30">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="R6" s="75"/>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="75"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="75"/>
+      <c r="Z6" s="75"/>
+      <c r="AA6" s="75"/>
+      <c r="AB6" s="75"/>
+      <c r="AC6" s="75"/>
     </row>
     <row r="7" spans="1:29">
       <c r="B7" s="13"/>
@@ -2649,10 +2830,13 @@
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="12"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
       <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
+      <c r="Q7" s="30">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="R7" s="12"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
@@ -2675,22 +2859,26 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="87" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="88"/>
-      <c r="H8" s="89"/>
+      <c r="F8" s="98" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="99"/>
+      <c r="H8" s="100"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="55" t="s">
-        <v>53</v>
-      </c>
-      <c r="O8" s="55"/>
+      <c r="N8" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="54"/>
+      <c r="Q8" s="30">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:29">
       <c r="B9" s="30"/>
@@ -2703,10 +2891,10 @@
         <v>17</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>6</v>
@@ -2715,26 +2903,30 @@
         <v>2</v>
       </c>
       <c r="N9" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="O9" s="56">
+        <v>38</v>
+      </c>
+      <c r="O9" s="55">
         <f>1024*1024*1024</f>
         <v>1073741824</v>
       </c>
+      <c r="Q9" s="30">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="90" t="s">
-        <v>134</v>
+      <c r="A10" s="101" t="s">
+        <v>126</v>
       </c>
       <c r="B10" s="31" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="35"/>
       <c r="E10" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="23">
         <f>6*0.85</f>
@@ -2744,34 +2936,41 @@
         <f>16*0.95</f>
         <v>15.2</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="25">
+        <f>40*0.975</f>
+        <v>39</v>
+      </c>
       <c r="I10" s="48">
         <f>IF(C$16=F$9,F10,IF(C$16=G$9,G10,H10))</f>
-        <v>15.2</v>
+        <v>39</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5">
         <v>3</v>
       </c>
       <c r="N10" s="53" t="s">
-        <v>40</v>
-      </c>
-      <c r="O10" s="56">
+        <v>39</v>
+      </c>
+      <c r="O10" s="55">
         <f>1000000000</f>
         <v>1000000000</v>
       </c>
+      <c r="Q10" s="30">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="91"/>
+      <c r="A11" s="102"/>
       <c r="B11" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>23</v>
+        <v>135</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="21">
         <v>1</v>
@@ -2780,17 +2979,15 @@
         <v>6</v>
       </c>
       <c r="H11" s="14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11" s="49">
-        <f t="shared" ref="I11:I12" si="0">IF(C$16=F$9,F11,IF(C$16=G$9,G11,H11))</f>
-        <v>6</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>22</v>
+        <f t="shared" ref="I11:I12" si="1">IF(C$16=F$9,F11,IF(C$16=G$9,G11,H11))</f>
+        <v>4</v>
+      </c>
+      <c r="Q11" s="30">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:29">
@@ -2799,11 +2996,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="35"/>
       <c r="E12" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="21">
         <v>31</v>
@@ -2811,20 +3008,29 @@
       <c r="G12" s="2">
         <v>420</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="14">
+        <f>256*0.9</f>
+        <v>230.4</v>
+      </c>
       <c r="I12" s="49">
-        <f t="shared" si="0"/>
-        <v>420</v>
-      </c>
-      <c r="K12" s="5"/>
+        <f t="shared" si="1"/>
+        <v>230.4</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="L12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N12" s="53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O12" s="53">
         <v>8</v>
+      </c>
+      <c r="Q12" s="30">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -2833,11 +3039,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="39">
-        <v>1000000</v>
+        <v>15360</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="22">
         <v>18688</v>
@@ -2845,16 +3051,20 @@
       <c r="G13" s="15">
         <v>4608</v>
       </c>
-      <c r="H13" s="16"/>
+      <c r="H13" s="16">
+        <v>1500</v>
+      </c>
       <c r="I13" s="49">
         <f>IF(C$16=F$9,F13,IF(C$16=G$9,G13,H13))</f>
-        <v>4608</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>3</v>
-      </c>
+        <v>1500</v>
+      </c>
+      <c r="K13" s="5"/>
       <c r="L13" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="Q13" s="30">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -2863,7 +3073,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="40">
-        <v>2000</v>
+        <v>1048576</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="12"/>
@@ -2871,22 +3081,25 @@
       <c r="G14" s="12"/>
       <c r="H14" s="13"/>
       <c r="I14" s="49"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5" t="s">
-        <v>25</v>
+      <c r="L14" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="N14" s="53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O14" s="53">
         <v>4</v>
+      </c>
+      <c r="Q14" s="30">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:29">
       <c r="B15" s="34"/>
       <c r="C15" s="41"/>
       <c r="E15" s="50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" s="45">
         <f>F11*F13</f>
@@ -2897,102 +3110,110 @@
         <v>27648</v>
       </c>
       <c r="H15" s="45">
-        <f>H10*O9</f>
-        <v>0</v>
+        <f>H11*H13</f>
+        <v>6000</v>
       </c>
       <c r="I15" s="49">
-        <f t="shared" ref="I15:I19" si="1">IF(C$16=F$9,F15,IF(C$16=G$9,G15,H15))</f>
-        <v>27648</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>16</v>
+        <f t="shared" ref="I15:I19" si="2">IF(C$16=F$9,F15,IF(C$16=G$9,G15,H15))</f>
+        <v>6000</v>
       </c>
       <c r="N15" s="53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O15" s="53">
         <v>8</v>
       </c>
+      <c r="Q15" s="30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:29">
-      <c r="A16" s="90" t="s">
-        <v>108</v>
+      <c r="A16" s="95" t="s">
+        <v>100</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="45">
         <f>F10*$O9</f>
         <v>5476083302.3999996</v>
       </c>
       <c r="G16" s="45">
-        <f t="shared" ref="G16:H16" si="2">G10*$O9</f>
+        <f>G10*$O9</f>
         <v>16320875724.799999</v>
       </c>
       <c r="H16" s="45">
+        <f>H10*$O9</f>
+        <v>41875931136</v>
+      </c>
+      <c r="I16" s="49">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="49">
-        <f t="shared" si="1"/>
-        <v>16320875724.799999</v>
-      </c>
-      <c r="K16" s="5"/>
+        <v>41875931136</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="L16" s="5" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="N16" s="53" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O16" s="53">
-        <f>IF(C17=L18,O14,O15)</f>
+        <f>IF(C17=L23,O14,O15)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="91"/>
+      <c r="Q16" s="30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="103"/>
       <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="45">
         <f>F12*$O9/F11</f>
         <v>33285996544</v>
       </c>
       <c r="G17" s="45">
-        <f t="shared" ref="G17:H17" si="3">G12*$O9/G11</f>
+        <f t="shared" ref="G17" si="3">G12*$O9/G11</f>
         <v>75161927680</v>
       </c>
       <c r="H17" s="45">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="H17" si="4">H12*$O9/H11</f>
+        <v>61847529062.400002</v>
       </c>
       <c r="I17" s="49">
-        <f t="shared" si="1"/>
-        <v>75161927680</v>
+        <f t="shared" si="2"/>
+        <v>61847529062.400002</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+        <v>24</v>
+      </c>
+      <c r="Q17" s="30">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="10"/>
       <c r="B18" s="32" t="s">
         <v>7</v>
@@ -3002,30 +3223,28 @@
       </c>
       <c r="D18" s="29"/>
       <c r="I18" s="49"/>
-      <c r="K18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="N18" s="53" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="O18" s="53">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="Q18" s="30">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="10"/>
       <c r="B19" s="32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="39">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F19" s="3">
         <f>100000000/30</f>
@@ -3036,15 +3255,21 @@
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="49">
-        <f t="shared" si="1"/>
-        <v>300000</v>
-      </c>
-      <c r="K19" s="5"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="L19" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="30">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="10"/>
       <c r="B20" s="32" t="s">
         <v>9</v>
@@ -3053,910 +3278,1656 @@
         <v>1</v>
       </c>
       <c r="D20" s="29"/>
-      <c r="K20" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="K20" s="5"/>
       <c r="L20" s="5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="N20" s="53" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O20" s="53">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="Q20" s="30">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="10"/>
       <c r="B21" s="32" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="39">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F21" s="2">
-        <f>IF(N36=1,F22,F25)</f>
+        <f>IF(N38=1,F22,F26)</f>
         <v>2.0579999999999998</v>
       </c>
       <c r="G21" s="2">
-        <f>IF(O36=1,G22,G25)</f>
-        <v>81.611000000000004</v>
+        <f>IF($O$38=1,G22,G26)</f>
+        <v>295.63299999999998</v>
+      </c>
+      <c r="H21" s="2">
+        <f>IF($O$38=1,H22,H26)</f>
+        <v>1687.5</v>
       </c>
       <c r="I21" s="48">
-        <f t="shared" ref="I21:I27" si="4">IF(C$16=F$9,F21,IF(C$16=G$9,G21,H21))</f>
-        <v>81.611000000000004</v>
+        <f t="shared" ref="I21:I23" si="5">IF(C$16=F$9,F21,IF(C$16=G$9,G21,H21))</f>
+        <v>1687.5</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="N21" s="53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O21" s="53">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="Q21" s="30">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="10"/>
       <c r="B22" s="32" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>34</v>
+        <v>136</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F22" s="6">
-        <f>IF(O36=1,F23,F24)</f>
-        <v>9.1080000000000005</v>
+        <f>IF(O38=1,F23,F24)</f>
+        <v>4.2889999999999997</v>
       </c>
       <c r="G22" s="6">
-        <f>IF(O34=1,G23,G24)</f>
+        <f>IF($O$34=1,G23,IF($O$34=2,G24,G25))</f>
         <v>295.63299999999998</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6">
+        <f>IF($O$34=1,H23,IF($O$34=2,H24,H25))</f>
+        <v>1687.5</v>
+      </c>
       <c r="I22" s="11">
-        <f t="shared" si="4"/>
-        <v>295.63299999999998</v>
-      </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5" t="s">
-        <v>27</v>
+        <f t="shared" si="5"/>
+        <v>1687.5</v>
       </c>
       <c r="N22" s="53" t="s">
-        <v>50</v>
+        <v>139</v>
       </c>
       <c r="O22" s="53">
-        <f>IF(C22=L24,O20,IF(C22=L25,O21,0))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+        <f>(1/O12)</f>
+        <v>0.125</v>
+      </c>
+      <c r="Q22" s="30">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="10"/>
       <c r="B23" s="32" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F23" s="6">
-        <f>IF(C17=L18,4.289,1.697)</f>
+        <f>IF(C17=L23,4.289,1.697)</f>
         <v>4.2889999999999997</v>
       </c>
       <c r="G23" s="6">
-        <f>IF(C17=L18,94.768,29.586)</f>
+        <f>IF($C$17=$L$23,94.768,29.586)</f>
         <v>94.768000000000001</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="11">
-        <f t="shared" si="4"/>
-        <v>94.768000000000001</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+        <v>15</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="O23" s="53">
+        <f>IF(C22=L31,O20,IF(C22=L32,O21,IF(C22=L33,O22,0)))</f>
+        <v>0.125</v>
+      </c>
+      <c r="Q23" s="30">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="10"/>
       <c r="B24" s="32" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="39">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F24" s="6">
         <f>9.108</f>
         <v>9.1080000000000005</v>
       </c>
       <c r="G24" s="6">
-        <f>IF(O35=1,295.633,IF(O32=1,71.587,104.37))</f>
+        <f>IF($O$37=1,295.633,IF($O$33=1,71.587,104.37))</f>
         <v>295.63299999999998</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I24:I29" si="6">IF(C$16=F$9,F24,IF(C$16=G$9,G24,H24))</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q24" s="30">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="10"/>
+      <c r="B25" s="85" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="86">
+        <v>1</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="6">
+        <f>IF($O$37=1,295.633,IF($O$33=1,71.587,104.37))</f>
         <v>295.63299999999998</v>
       </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="53" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="O24" s="53">
+      <c r="H25" s="6">
+        <v>1687.5</v>
+      </c>
+      <c r="I25" s="11">
+        <f t="shared" si="6"/>
+        <v>1687.5</v>
+      </c>
+      <c r="N25" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="O25" s="53">
         <f>O15</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="10"/>
-      <c r="B25" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="40">
-        <v>280</v>
-      </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="6">
-        <f>IF(O34=1,F26,F27)</f>
+      <c r="Q25" s="30">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="10"/>
+      <c r="B26" s="87" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="88">
+        <v>1000</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="6">
+        <f>IF(O34=1,F27,F28)</f>
         <v>2.0579999999999998</v>
       </c>
-      <c r="G25" s="6">
-        <f>IF(O34=1,G26,G27)</f>
-        <v>81.611000000000004</v>
-      </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="11">
-        <f t="shared" si="4"/>
-        <v>81.611000000000004</v>
-      </c>
-      <c r="K25" s="5"/>
-      <c r="L25" s="53" t="s">
-        <v>35</v>
-      </c>
-      <c r="N25" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="O25" s="53">
+      <c r="G26" s="6">
+        <f>IF($O$34=1,G27,IF($O$35=1,G28,G29))</f>
+        <v>132.9127</v>
+      </c>
+      <c r="H26" s="6">
+        <f>IF($O$34=1,H27,IF($O$35=1,H28,H29))</f>
+        <v>843.75</v>
+      </c>
+      <c r="I26" s="11">
+        <f t="shared" si="6"/>
+        <v>843.75</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N26" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="O26" s="53">
         <f>2*O15</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="B26" s="34"/>
-      <c r="C26" s="41"/>
-      <c r="E26" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" s="6">
-        <f>IF(C17=L18,5.695,2.445)</f>
+      <c r="Q26" s="30">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="B27" s="34"/>
+      <c r="C27" s="41"/>
+      <c r="E27" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="6">
+        <f>IF(C17=L23,5.695,2.445)</f>
         <v>5.6950000000000003</v>
       </c>
-      <c r="G26" s="6">
-        <f>IF(C17=L18,72.499,27.755)</f>
+      <c r="G27" s="6">
+        <f>IF($C$17=$L$23,72.499,27.755)</f>
         <v>72.498999999999995</v>
       </c>
-      <c r="H26" s="6"/>
-      <c r="I26" s="11">
-        <f t="shared" si="4"/>
-        <v>72.498999999999995</v>
-      </c>
-      <c r="K26" s="6"/>
-      <c r="L26" s="53"/>
-      <c r="N26" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="O26" s="53">
-        <f>IF(C10=L9,O24,O25)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="10"/>
-      <c r="B27" s="95" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" s="94">
+      <c r="H27" s="6"/>
+      <c r="I27" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="O27" s="53">
+        <f>IF(C10=L9,O25,O26)</f>
+        <v>8</v>
+      </c>
+      <c r="Q27" s="30">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="10"/>
+      <c r="B28" s="84" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="83">
         <v>0.1</v>
       </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="D28" s="29"/>
+      <c r="E28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="6">
         <f>2.058</f>
         <v>2.0579999999999998</v>
       </c>
-      <c r="G27" s="6">
-        <f>IF(O35=1,81.611,IF(O32=1,21.163,23.672))</f>
-        <v>81.611000000000004</v>
-      </c>
-      <c r="H27" s="6"/>
-      <c r="I27" s="11">
-        <f t="shared" si="4"/>
-        <v>81.611000000000004</v>
-      </c>
-      <c r="L27" s="53"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="B28" s="13" t="s">
+      <c r="G28" s="6">
+        <f>IF($O$37=1,132.9127,IF($O$33=1,21.163,23.672))</f>
+        <v>132.9127</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q28" s="30">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="B29" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="80">
+        <f>O62*10*C14</f>
+        <v>0.62495129599999999</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="81">
-        <f>O55*10*C14</f>
-        <v>1.1919999999999999E-3</v>
-      </c>
-      <c r="L28" s="54"/>
-      <c r="N28" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="O28" s="53">
-        <f>IF(C11=L11,O16,IF(O35=1,O22,2*O15))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="B29" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C29" s="42">
-        <f>C28/C27</f>
-        <v>1.1919999999999998E-2</v>
-      </c>
-      <c r="L29" s="53"/>
+      <c r="G29" s="6">
+        <f>IF($O$37=1,132.9127,IF($O$33=1,21.163,23.672))</f>
+        <v>132.9127</v>
+      </c>
+      <c r="H29" s="6">
+        <v>843.75</v>
+      </c>
+      <c r="I29" s="11">
+        <f t="shared" si="6"/>
+        <v>843.75</v>
+      </c>
       <c r="N29" s="53" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="O29" s="53">
-        <f>IF(C11=L11,O16,IF(O35=1,4,2*O15))</f>
+        <f>IF(C11=L12,O16,IF(O37=1,O23,2*O15))</f>
+        <v>0.125</v>
+      </c>
+      <c r="Q29" s="30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="B30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="42">
+        <f>C29/C28</f>
+        <v>6.2495129599999997</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L30" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="N30" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="O30" s="53">
+        <f>IF(C11=L12,O16,IF(O37=1,4,2*O15))</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="B30" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30" s="3">
-        <f>CEILING(O53,POWER(2,O38))/POWER(2,O38)-1</f>
-        <v>8388607</v>
-      </c>
-      <c r="L30" s="53"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="Q30" s="30">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="B31" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="83">
-        <f>C14/C30</f>
-        <v>2.3841860752327532E-4</v>
-      </c>
-      <c r="L31" s="53"/>
-      <c r="N31" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="O31" s="53">
+        <v>127</v>
+      </c>
+      <c r="C31" s="3">
+        <f>CEILING(O60,POWER(2,O40))/POWER(2,O40)-1</f>
+        <v>16777215</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q31" s="30">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="B32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="82">
+        <f>C14/C31</f>
+        <v>6.2500003725290521E-2</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="L32" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="N32" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="O32" s="53">
         <f>IF(C20&gt;1,1,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="B32" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" s="2">
-        <f>IF(C16=L15,0,O40)</f>
-        <v>2</v>
-      </c>
-      <c r="L32" s="53"/>
-      <c r="N32" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="O32" s="53">
-        <f>IF(C12=L14,1,0)</f>
+      <c r="Q32" s="30">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17">
+      <c r="B33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="2">
+        <f>IF(C16=L19,0,O42)</f>
+        <v>5</v>
+      </c>
+      <c r="K33" s="6"/>
+      <c r="L33" s="53" t="s">
+        <v>136</v>
+      </c>
+      <c r="N33" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="O33" s="53">
+        <f>IF(C12=L17,1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:15">
-      <c r="B33" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="45">
-        <f>IF(O36=1,1+FLOOR(C19,2)/2,(C19+1)*(C19+2)/2)</f>
-        <v>5151</v>
-      </c>
-      <c r="L33" s="53"/>
-      <c r="N33" s="53" t="s">
+      <c r="Q33" s="30">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17">
+      <c r="B34" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="45">
+        <f>IF(O38=1,1+FLOOR(C19,2)/2,(C19+1)*(C19+2)/2)</f>
+        <v>1</v>
+      </c>
+      <c r="L34" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="N34" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="O33" s="53">
+      <c r="O34" s="53">
         <f>IF(C11=L12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="30">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17">
+      <c r="B35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="42">
+        <f>C24/C34</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15">
-      <c r="B34" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="42">
-        <f>C24/C33</f>
-        <v>2.5237817899437003E-2</v>
-      </c>
-      <c r="L34" s="53"/>
-      <c r="N34" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="O34" s="53">
-        <f>1-O33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15">
-      <c r="B35" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="44">
-        <f>IF(O36=1,1,O42)</f>
-        <v>1E+30</v>
       </c>
       <c r="L35" s="53"/>
       <c r="N35" s="53" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="O35" s="53">
-        <f>IF(C22=L23,0,1)</f>
+        <f>IF(C11=L13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q35" s="30">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17">
+      <c r="B36" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="44">
+        <f>IF(O38=1,1,O49)</f>
         <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15">
-      <c r="B36" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="42">
-        <f>C25/C35</f>
-        <v>2.7999999999999998E-28</v>
       </c>
       <c r="L36" s="53"/>
       <c r="N36" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="O36" s="56">
-        <f>IF(C10=L9,1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15">
+        <v>142</v>
+      </c>
+      <c r="O36" s="53">
+        <f>IF(C11=L14,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q36" s="30">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17">
       <c r="B37" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="61">
-        <f>IF(O36=1,(1+FLOOR(C19,2)/2)/C21/C24,(C19+1)*(C19+2)/C21/C24)</f>
-        <v>0.99057692307692313</v>
+        <v>132</v>
+      </c>
+      <c r="C37" s="42">
+        <f>C25/C36</f>
+        <v>1</v>
       </c>
       <c r="L37" s="53"/>
       <c r="N37" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="O37" s="56">
-        <f>IF(C10=L10,1,0)</f>
+        <v>79</v>
+      </c>
+      <c r="O37" s="53">
+        <f>IF(C22=L30,0,1)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="2:15">
+      <c r="Q37" s="30">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17">
       <c r="B38" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C38" s="42">
-        <f>(CEILING(C37,1)-C37)/C37</f>
-        <v>9.5127159774800445E-3</v>
+        <v>103</v>
+      </c>
+      <c r="C38" s="60">
+        <f>IF(O38=1,(1+FLOOR(C19,2)/2)/C21/C24,(C19+1)*(C19+2)/C21/C24)</f>
+        <v>1</v>
       </c>
       <c r="L38" s="53"/>
       <c r="N38" s="53" t="s">
+        <v>85</v>
+      </c>
+      <c r="O38" s="55">
+        <f>IF(C10=L9,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q38" s="30">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17">
+      <c r="B39" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="42">
+        <f>(CEILING(C38,1)-C38)/C38</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="53"/>
+      <c r="N39" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="O39" s="55">
+        <f>IF(C10=L10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q39" s="30">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17">
+      <c r="B40" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="60" t="str">
+        <f>IF(O39=1,C78/6/C25,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="N40" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="O38" s="53">
-        <f>O36*2+O37*3</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15">
-      <c r="B39" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="61">
-        <f>IF(O37=1,C77/6/C25,"N/A")</f>
-        <v>5.9571428571428573</v>
-      </c>
-      <c r="N39" s="53" t="s">
+      <c r="O40" s="53">
+        <f>O38*2+O39*3</f>
+        <v>2</v>
+      </c>
+      <c r="Q40" s="30">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17">
+      <c r="N41" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="O39" s="53">
-        <f>IF(C22=L23,0,IF(C22=L24,1,2))</f>
+      <c r="O41" s="53">
+        <f>IF(C22=L30,0,IF(C22=L31,1,2))</f>
+        <v>2</v>
+      </c>
+      <c r="Q41" s="30">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17">
+      <c r="B42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="3">
+        <f>O37*2*(CEILING(C79,C23)/C23)*(2*C77)*O23</f>
+        <v>2013265920</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="N42" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="O42" s="53">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="30">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17">
+      <c r="B43" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="3">
+        <f>IF(O38=1,L99+L100+L101+L102+L103,"N/A")</f>
+        <v>32967536640</v>
+      </c>
+      <c r="E43" s="2">
+        <f>IF(O38=1,3*C82+(2+O32)*C83+C42+IF(O43=1,C77*C77*4*(4+8),0),"N/A")</f>
+        <v>32967229440</v>
+      </c>
+      <c r="N43" s="53" t="s">
+        <v>144</v>
+      </c>
+      <c r="O43" s="53">
+        <f>O37</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="2:15">
-      <c r="N40" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="O40" s="53">
+      <c r="Q43" s="30">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17">
+      <c r="B44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="3" t="str">
+        <f>IF(O39=1,L97+L98+L99+L100,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="E44" s="2" t="str">
+        <f>IF(O39=1,(3*C82)+(2*C82+2*C83+O32*2*C83+O34*3*C83)+C42+IF(O43=1,C77*C77*4*(4+8)-2*C82,0), "N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="N44" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="O44" s="53">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="30">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17">
+      <c r="B45" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="3">
+        <f>IF(O38=1,C43,C44)</f>
+        <v>32967536640</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="N45" s="53" t="s">
+        <v>155</v>
+      </c>
+      <c r="O45" s="53">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="30">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17">
+      <c r="B46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="42">
+        <f>C45/I16</f>
+        <v>0.78726695134089542</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="N46" s="53" t="s">
+        <v>161</v>
+      </c>
+      <c r="O46" s="53">
+        <f>IF(C22=L33,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q46" s="30">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17">
+      <c r="B47" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="42">
+        <f>C45/I16</f>
+        <v>0.78726695134089542</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="N47" s="53" t="s">
+        <v>162</v>
+      </c>
+      <c r="O47" s="53">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="30">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17">
+      <c r="E48" s="2"/>
+      <c r="Q48" s="30">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:17">
+      <c r="B49" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="3">
+        <f>IF(O38=1,K99+K100+K101+K102+K103,"N/A")</f>
+        <v>34999554048</v>
+      </c>
+      <c r="E49" s="2">
+        <f>IF(O38=1,C82+(C43-C42)+2*C86+C89+IF(O43=1,C77*C77*C494*(4+8),0),"N/A")</f>
+        <v>34984700313.599998</v>
+      </c>
+      <c r="N49" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="O49" s="56">
+        <v>1E+30</v>
+      </c>
+      <c r="Q49" s="30">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:17">
+      <c r="B50" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="3" t="str">
+        <f>IF(O39=1,K97+K98+K99+K101+K102,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="E50" s="2" t="str">
+        <f>IF(O39=1,C82+(C44-C42)+3*C86+C89+4*C82,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="Q50" s="30">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:17">
+      <c r="B51" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="3">
+        <f>IF(O38=1,C49,C50)</f>
+        <v>34999554048</v>
+      </c>
+      <c r="D51" s="29"/>
+      <c r="E51" s="2"/>
+      <c r="N51" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="O51" s="55">
+        <f>IF(O34=1,O12*O16,2)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="2:15">
-      <c r="B41" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="3">
-        <f>O35*2*(CEILING(C78,C23)/C23)*(2*C76)*O22</f>
-        <v>160032000</v>
-      </c>
-    </row>
-    <row r="42" spans="2:15">
-      <c r="B42" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C42" s="3" t="str">
-        <f>IF(O36=1,3*C81+(2+O31)*C82+C41,"N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="N42" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="O42" s="57">
-        <v>1E+30</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15">
-      <c r="B43" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="3">
-        <f>O37*((3*C81)+(2*C81+2*C82+O31*2*C82+O34*3*C82)+C41)</f>
-        <v>3386317128</v>
-      </c>
-    </row>
-    <row r="44" spans="2:15">
-      <c r="B44" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="3">
-        <f>IF(O36=1,C42,C43)</f>
-        <v>3386317128</v>
-      </c>
-      <c r="N44" s="53" t="s">
+      <c r="Q51" s="30">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="O44" s="56">
-        <f>IF(O33=1,2,O12*O16)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15">
-      <c r="B45" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="42">
-        <f>C44/I16</f>
-        <v>0.20748378856009558</v>
-      </c>
-      <c r="N45" s="53" t="s">
+    </row>
+    <row r="52" spans="2:17">
+      <c r="B52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="42">
+        <f>C51/I17</f>
+        <v>0.5659006039301554</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="N52" s="53" t="s">
+        <v>165</v>
+      </c>
+      <c r="O52" s="55">
+        <f>IF(O34=1,O16,POWER(2,O40)*O15/2)</f>
+        <v>16</v>
+      </c>
+      <c r="Q52" s="30">
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="O45" s="56">
-        <f>IF(O34=1,O16,O15*POWER(2,O38)/2)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="2:15">
-      <c r="B46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C46" s="42">
-        <f>C44/I16</f>
-        <v>0.20748378856009558</v>
-      </c>
-      <c r="N46" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="O46" s="53">
+    </row>
+    <row r="53" spans="2:17">
+      <c r="N53" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="O53" s="53">
         <f>IF(O34=1,O16,O15*POWER(2,2)/2)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="2:15">
-      <c r="N47" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="O47" s="56">
+      <c r="Q53" s="30">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17">
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="3">
+        <f>C19*C20*C21</f>
+        <v>1</v>
+      </c>
+      <c r="N54" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="O54" s="55">
         <f>O18</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="48" spans="2:15">
-      <c r="B48" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="3" t="str">
-        <f>IF(O36=1,C81+(C42-C41)+2*C85+C88,"N/A")</f>
+      <c r="Q54" s="30">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17">
+      <c r="B55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="36">
+        <f>CEILING(C54,I11)</f>
+        <v>4</v>
+      </c>
+      <c r="N55" s="53" t="s">
+        <v>52</v>
+      </c>
+      <c r="O55" s="55">
+        <f>IF(O34=1,0,O27)</f>
+        <v>8</v>
+      </c>
+      <c r="Q55" s="30">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17">
+      <c r="B56" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="81">
+        <f>C55/I11</f>
+        <v>1</v>
+      </c>
+      <c r="N56" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="O56" s="55">
+        <f>IF(O33=1, O55,0)</f>
+        <v>8</v>
+      </c>
+      <c r="Q56" s="30">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17">
+      <c r="B57" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="80">
+        <f>C56/I13</f>
+        <v>6.6666666666666664E-4</v>
+      </c>
+      <c r="N57" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="O57" s="55">
+        <f>O52+O54+O55+O56</f>
+        <v>40</v>
+      </c>
+      <c r="Q57" s="30">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17">
+      <c r="B58" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="42">
+        <f>C57/0.2</f>
+        <v>3.3333333333333331E-3</v>
+      </c>
+      <c r="Q58" s="30">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17">
+      <c r="N59" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="O59" s="53">
+        <v>26</v>
+      </c>
+      <c r="Q59" s="30">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17">
+      <c r="B60" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="3">
+        <f>IF(O37=1,CEILING(C79,C23)/C23,IF(O35=0,C79,CEILING(C79,64)/64))</f>
+        <v>262144</v>
+      </c>
+      <c r="N60" s="53" t="s">
+        <v>129</v>
+      </c>
+      <c r="O60" s="55">
+        <f>POWER(2,O59)</f>
+        <v>67108864</v>
+      </c>
+      <c r="Q60" s="30">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17">
+      <c r="B61" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="3">
+        <f>C77*(1+O37)</f>
+        <v>30720</v>
+      </c>
+      <c r="Q61" s="30">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17">
+      <c r="B62" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="43">
+        <f>MAX(C60/C61,C61/C60)</f>
+        <v>8.5333333333333332</v>
+      </c>
+      <c r="N62" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="O62" s="53">
+        <f>IF(C17=L23,0.0000000596,0.000000000000000111)</f>
+        <v>5.9599999999999998E-8</v>
+      </c>
+      <c r="Q62" s="30">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17">
+      <c r="B63" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="3">
+        <f>2*C60*C61*O29+C61*C61*O30</f>
+        <v>5788139520</v>
+      </c>
+      <c r="Q63" s="30">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17">
+      <c r="N64" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="O64" s="53">
+        <f>IF(O43=0,O57,O54+O30)</f>
+        <v>12</v>
+      </c>
+      <c r="Q64" s="30">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="B65" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="3">
+        <f>IF(O38=1,CEILING(CEILING(CEILING(C19+1,2)/2,C21)/C21,C24)/C24,"N/A")</f>
+        <v>1</v>
+      </c>
+      <c r="N65" s="53" t="s">
+        <v>164</v>
+      </c>
+      <c r="O65" s="53">
+        <f>IF(O43=0,1,POWER(2,O40))</f>
+        <v>4</v>
+      </c>
+      <c r="Q65" s="30">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="B66" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" s="3" t="str">
+        <f>IF(O39=1,CEILING((C19+1)*(C19+2),C21*C24)/(C21*C24),"N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="N48" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="O48" s="56">
-        <f>IF(O33=1,O26,0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15">
-      <c r="B49" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="3">
-        <f>IF(O37=1,C81+(C43-C41)+3*C85+C88,"N/A")</f>
-        <v>46448807904</v>
-      </c>
-      <c r="N49" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="O49" s="56">
-        <f>IF(O32=1, O48,0)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15">
-      <c r="B50" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C50" s="3">
-        <f>IF(O36=1,C48,C49)</f>
-        <v>46448807904</v>
-      </c>
-      <c r="D50" s="29"/>
-      <c r="N50" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="O50" s="56">
-        <f>O45+O47+O48+O49</f>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="2:15">
-      <c r="B51" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51" s="42">
-        <f>C50/I17</f>
-        <v>0.61798319092818665</v>
-      </c>
-    </row>
-    <row r="52" spans="2:15">
-      <c r="N52" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="O52" s="53">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="2:15">
-      <c r="B53" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C53" s="3">
-        <f>C19*C20*C21</f>
-        <v>8000</v>
-      </c>
-      <c r="N53" s="53" t="s">
-        <v>137</v>
-      </c>
-      <c r="O53" s="56">
-        <f>POWER(2,O52)</f>
-        <v>67108864</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15">
-      <c r="B54" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C54" s="36">
-        <f>CEILING(C53,I11)</f>
-        <v>8004</v>
-      </c>
-    </row>
-    <row r="55" spans="2:15">
-      <c r="B55" s="79" t="s">
-        <v>117</v>
-      </c>
-      <c r="C55" s="82">
-        <f>C54/I11</f>
-        <v>1334</v>
-      </c>
-      <c r="N55" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="O55" s="53">
-        <f>IF(C17=L18,0.0000000596,0.000000000000000111)</f>
-        <v>5.9599999999999998E-8</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15">
-      <c r="B56" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C56" s="81">
-        <f>C55/I13</f>
-        <v>0.28949652777777779</v>
-      </c>
-    </row>
-    <row r="57" spans="2:15">
-      <c r="B57" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C57" s="42">
-        <f>C56/0.2</f>
-        <v>1.4474826388888888</v>
-      </c>
-    </row>
-    <row r="59" spans="2:15">
-      <c r="B59" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="3">
-        <f>IF(O35=1,CEILING(C78,C23)/C23,IF(O33=0,C78,CEILING(C78,64)/64))</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="60" spans="2:15">
-      <c r="B60" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" s="3">
-        <f>C76*(1+O35)</f>
-        <v>20004</v>
-      </c>
-    </row>
-    <row r="61" spans="2:15">
-      <c r="B61" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C61" s="43">
-        <f>MAX(C59/C60,C60/C59)</f>
-        <v>10.002000000000001</v>
-      </c>
-    </row>
-    <row r="62" spans="2:15">
-      <c r="B62" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C62" s="3">
-        <f>2*C59*C60*O28+C60*C60*O29</f>
-        <v>1760672064</v>
-      </c>
-    </row>
-    <row r="64" spans="2:15">
-      <c r="B64" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C64" s="3" t="str">
-        <f>IF(O36=1,CEILING(CEILING(CEILING(C19+1,2)/2,C21)/C21,C24)/C24,"N/A")</f>
+      <c r="Q66" s="30">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="B67" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" s="3" t="str">
+        <f>IF(O39=1,C84,"N/A")</f>
         <v>N/A</v>
       </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="B65" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C65" s="3">
-        <f>IF(O37=1,CEILING((C19+1)*(C19+2),C21*C24)/(C21*C24),"N/A")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="B66" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="3">
-        <f>IF(O37=1,C83,"N/A")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="D67" s="29"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="B68" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C68" s="46">
-        <f>IF(O36=1,C14*C13*C13/2,C14*C13*C13*C13/6)</f>
-        <v>3.3333333333333331E+20</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="B69" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C69" s="58">
+      <c r="Q67" s="30">
+        <f t="shared" ref="Q67:Q90" si="7">Q66+1</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="D68" s="29"/>
+      <c r="Q68" s="30">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="B69" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="46">
+        <f>IF(O38=1,C14*C13*C13/2,C14*C13*C13*C13/6)</f>
+        <v>123695058124800</v>
+      </c>
+      <c r="Q69" s="30">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="B70" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" s="57">
         <f>I21*1000000000000000</f>
-        <v>8.1611E+16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="B70" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="C70" s="59">
+        <v>1.6875E+18</v>
+      </c>
+      <c r="Q70" s="30">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="B71" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" s="58">
         <f>1.75/82</f>
         <v>2.1341463414634148E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="92" t="s">
-        <v>132</v>
-      </c>
-      <c r="B71" s="13" t="s">
+      <c r="Q71" s="30">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="A72" s="104" t="s">
+        <v>124</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" s="79">
+        <f>C70*C71</f>
+        <v>3.6013719512195124E+16</v>
+      </c>
+      <c r="Q72" s="30">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="A73" s="105"/>
+      <c r="B73" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="C73" s="89">
+        <f>C69/C72/3600*I13</f>
+        <v>1.4311103726608251E-3</v>
+      </c>
+      <c r="E73" s="51"/>
+      <c r="Q73" s="30">
+        <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="B74" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C74" s="80" t="e">
+        <f>C73/I19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q74" s="30">
+        <f t="shared" si="7"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="C75" s="1"/>
+      <c r="G75" s="52"/>
+      <c r="Q75" s="30">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="Q76" s="30">
+        <f t="shared" si="7"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
+      <c r="A77" s="10"/>
+      <c r="B77" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="3">
+        <f>CEILING(CEILING(C13,C19)/C19,IF(O39=1,6,1))</f>
+        <v>15360</v>
+      </c>
+      <c r="D77" s="29"/>
+      <c r="Q77" s="30">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
+      <c r="B78" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C71" s="80">
-        <f>C69*C70</f>
-        <v>1741698170731707.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="93"/>
-      <c r="B72" s="79" t="s">
-        <v>122</v>
-      </c>
-      <c r="C72" s="82">
-        <f>C68/C71/3600*I13</f>
-        <v>244971.6453956078</v>
-      </c>
-      <c r="E72" s="51"/>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="B73" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C73" s="81">
-        <f>C72/I19</f>
-        <v>0.81657215131869265</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="C74" s="1"/>
-      <c r="G74" s="52"/>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="10"/>
-      <c r="B76" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C76" s="3">
-        <f>CEILING(CEILING(C13,C19)/C19,IF(O37=1,6,1))</f>
-        <v>10002</v>
-      </c>
-      <c r="D76" s="29"/>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="B77" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C77" s="3">
-        <f>IF(AND(O35=0,O37=0),C76,IF(O35=0,CEILING(C76,6),IF(O37=0,CEILING(C76,4),CEILING(C76,24))))</f>
-        <v>10008</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="B78" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C78" s="3">
+        <f>IF(AND(O37=0,O39=0),C77,IF(O37=0,CEILING(C77,6),IF(O39=0,CEILING(C77,4),CEILING(C77,24))))</f>
+        <v>15360</v>
+      </c>
+      <c r="Q78" s="30">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17">
+      <c r="B79" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" s="3">
         <f>CEILING(C14,C20)/C20</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="B80" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" s="3">
-        <f>CEILING(C78*O44,O12)/O12</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3">
+        <v>1048576</v>
+      </c>
+      <c r="Q79" s="30">
+        <f t="shared" si="7"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17">
+      <c r="Q80" s="30">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17">
       <c r="B81" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C81" s="3">
-        <f>C80*C76</f>
-        <v>5001000</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3">
+        <f>CEILING(C79*O51,O12)/O12</f>
+        <v>262144</v>
+      </c>
+      <c r="Q81" s="30">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17">
       <c r="B82" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C82" s="3">
-        <f>O46*C76*C76</f>
-        <v>1600640064</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3">
+        <f>C81*C77</f>
+        <v>4026531840</v>
+      </c>
+      <c r="Q82" s="30">
+        <f t="shared" si="7"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17">
       <c r="B83" s="2" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="C83" s="3">
-        <f>CEILING(C76,6*C25)/(6*C25)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3">
+        <f>O53*C77*C77</f>
+        <v>3774873600</v>
+      </c>
+      <c r="Q83" s="30">
+        <f t="shared" si="7"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17">
       <c r="B84" s="2" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="C84" s="3">
-        <f>O50*C76*C76*C83</f>
-        <v>43217281728</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3">
+        <f>CEILING(C77,6*C25)/(6*C25)</f>
+        <v>2560</v>
+      </c>
+      <c r="Q84" s="30">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17">
       <c r="B85" s="2" t="s">
-        <v>74</v>
+        <v>172</v>
       </c>
       <c r="C85" s="3">
-        <f>C76*O16*IF(O36=1,1,(1+O31)*(1+O32))</f>
-        <v>80016</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3">
+        <f>O64*C77*C77*C84</f>
+        <v>7247757312000</v>
+      </c>
+      <c r="Q85" s="30">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17">
       <c r="B86" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C86" s="3" t="str">
-        <f>IF(O36=1,C82*C64,"N/A")</f>
+        <v>69</v>
+      </c>
+      <c r="C86" s="3">
+        <f>C77*O16*IF(O38=1,1,(1+O32)*(1+O33))</f>
+        <v>61440</v>
+      </c>
+      <c r="Q86" s="30">
+        <f t="shared" si="7"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
+      <c r="B87" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="3">
+        <f>IF(O38=1,C83*C65/C26,"N/A")</f>
+        <v>3774873.6000000001</v>
+      </c>
+      <c r="Q87" s="30">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17">
+      <c r="B88" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C88" s="3" t="str">
+        <f>IF(O39=1,C85*C66/C26,"N/A")</f>
         <v>N/A</v>
       </c>
-    </row>
-    <row r="87" spans="2:3">
-      <c r="B87" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C87" s="3">
-        <f>IF(O37=1,C84*C65,"N/A")</f>
-        <v>43217281728</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3">
-      <c r="B88" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C88" s="3">
-        <f>IF(O36=1,C86,C87)</f>
-        <v>43217281728</v>
-      </c>
+      <c r="Q88" s="30">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17">
+      <c r="B89" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" s="3">
+        <f>IF(O38=1,C87,C88)</f>
+        <v>3774873.6000000001</v>
+      </c>
+      <c r="Q89" s="30">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17">
+      <c r="B90" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C90" s="3">
+        <f>IF(O38=1,C65*C78*C78,"N/A")</f>
+        <v>235929600</v>
+      </c>
+      <c r="Q90" s="30">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17">
+      <c r="B91" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C91" s="3" t="str">
+        <f>IF(O39=1,C84*C78*C78,"N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17">
+      <c r="B92" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C92" s="3">
+        <f>IF(O38=1,C90,C91)</f>
+        <v>235929600</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17">
+      <c r="B93" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C93" s="3">
+        <f>IF(O43=0,B92*(O52+O54),C92*O65*(O64+O54))/C26</f>
+        <v>18874368</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17">
+      <c r="A96" s="92" t="s">
+        <v>151</v>
+      </c>
+      <c r="E96" s="94" t="s">
+        <v>146</v>
+      </c>
+      <c r="F96" s="94" t="s">
+        <v>147</v>
+      </c>
+      <c r="G96" s="94" t="s">
+        <v>148</v>
+      </c>
+      <c r="H96" s="94" t="s">
+        <v>157</v>
+      </c>
+      <c r="I96" s="94" t="s">
+        <v>158</v>
+      </c>
+      <c r="J96" s="92"/>
+      <c r="K96" s="94" t="s">
+        <v>149</v>
+      </c>
+      <c r="L96" s="94" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97" s="90" t="s">
+        <v>145</v>
+      </c>
+      <c r="E97" s="2">
+        <v>4</v>
+      </c>
+      <c r="F97" s="2">
+        <v>3</v>
+      </c>
+      <c r="G97" s="2"/>
+      <c r="H97" s="3">
+        <f>3 * C86</f>
+        <v>184320</v>
+      </c>
+      <c r="I97" s="3">
+        <f>H97</f>
+        <v>184320</v>
+      </c>
+      <c r="J97" s="91"/>
+      <c r="K97" s="3">
+        <f t="shared" ref="K97:K103" si="8">E97*C$82+F97*C$82+G97*C$83+H97</f>
+        <v>28185907200</v>
+      </c>
+      <c r="L97" s="3">
+        <f t="shared" ref="L97:L103" si="9">F97*C$82+G97*C$83+I97</f>
+        <v>12079779840</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" s="90" t="s">
+        <v>152</v>
+      </c>
+      <c r="E98" s="2"/>
+      <c r="G98" s="2">
+        <f>2*(O32*1+1)+O34*3</f>
+        <v>2</v>
+      </c>
+      <c r="H98" s="3">
+        <f>2*(C81*IF(O44=1,1,C78))</f>
+        <v>524288</v>
+      </c>
+      <c r="I98" s="3">
+        <f>H98</f>
+        <v>524288</v>
+      </c>
+      <c r="J98" s="91"/>
+      <c r="K98" s="3">
+        <f t="shared" si="8"/>
+        <v>7550271488</v>
+      </c>
+      <c r="L98" s="3">
+        <f t="shared" si="9"/>
+        <v>7550271488</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" s="90" t="s">
+        <v>153</v>
+      </c>
+      <c r="E99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="3">
+        <f>IF(O45=1,C78*C78*4*(4+8),0)</f>
+        <v>11324620800</v>
+      </c>
+      <c r="I99" s="3">
+        <f>H99</f>
+        <v>11324620800</v>
+      </c>
+      <c r="J99" s="91"/>
+      <c r="K99" s="3">
+        <f t="shared" si="8"/>
+        <v>11324620800</v>
+      </c>
+      <c r="L99" s="3">
+        <f t="shared" si="9"/>
+        <v>11324620800</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
+      <c r="A100" s="90" t="s">
+        <v>156</v>
+      </c>
+      <c r="E100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3">
+        <f>O37*(2*2*C78*C79*O29/C23+O46*C78*2*4)</f>
+        <v>2013388800</v>
+      </c>
+      <c r="J100" s="91"/>
+      <c r="K100" s="3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L100" s="3">
+        <f t="shared" si="9"/>
+        <v>2013388800</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
+      <c r="A101" s="90" t="s">
+        <v>159</v>
+      </c>
+      <c r="E101" s="2">
+        <v>1</v>
+      </c>
+      <c r="G101" s="2"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="91"/>
+      <c r="K101" s="3">
+        <f t="shared" si="8"/>
+        <v>4026531840</v>
+      </c>
+      <c r="L101" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12">
+      <c r="A102" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="G102" s="2"/>
+      <c r="H102" s="3">
+        <f>C93+IF(O47=1,0,C92*(O55+O56))</f>
+        <v>18874368</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="91"/>
+      <c r="K102" s="3">
+        <f t="shared" si="8"/>
+        <v>18874368</v>
+      </c>
+      <c r="L102" s="3">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12">
+      <c r="A103" s="93" t="s">
+        <v>174</v>
+      </c>
+      <c r="F103" s="2">
+        <v>3</v>
+      </c>
+      <c r="G103" s="2">
+        <f>2+O32*1</f>
+        <v>2</v>
+      </c>
+      <c r="H103" s="3">
+        <f>3 * C86</f>
+        <v>184320</v>
+      </c>
+      <c r="I103" s="3">
+        <f>H103</f>
+        <v>184320</v>
+      </c>
+      <c r="J103" s="91"/>
+      <c r="K103" s="3">
+        <f t="shared" si="8"/>
+        <v>19629527040</v>
+      </c>
+      <c r="L103" s="3">
+        <f>F103*C$82+G103*C$83+I103</f>
+        <v>19629527040</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
+      <c r="A104" s="90"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="91"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+    </row>
+    <row r="105" spans="1:12">
+      <c r="A105" s="90"/>
+      <c r="G105" s="2"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="91"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+    </row>
+    <row r="106" spans="1:12">
+      <c r="A106" s="90"/>
+      <c r="G106" s="2"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="91"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+    </row>
+    <row r="107" spans="1:12">
+      <c r="A107" s="90"/>
+      <c r="G107" s="2"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="91"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+    </row>
+    <row r="108" spans="1:12">
+      <c r="A108" s="90"/>
+      <c r="G108" s="2"/>
+      <c r="I108" s="3"/>
+      <c r="J108" s="91"/>
+      <c r="K108" s="3"/>
+      <c r="L108" s="3"/>
+    </row>
+    <row r="109" spans="1:12">
+      <c r="A109" s="90"/>
+      <c r="G109" s="2"/>
+      <c r="I109" s="3"/>
+      <c r="J109" s="91"/>
+      <c r="K109" s="3"/>
+      <c r="L109" s="3"/>
+    </row>
+    <row r="110" spans="1:12">
+      <c r="A110" s="90"/>
+      <c r="G110" s="2"/>
+      <c r="I110" s="3"/>
+      <c r="J110" s="91"/>
+      <c r="K110" s="3"/>
+      <c r="L110" s="3"/>
+    </row>
+    <row r="111" spans="1:12">
+      <c r="A111" s="90"/>
+      <c r="G111" s="2"/>
+      <c r="I111" s="3"/>
+      <c r="J111" s="91"/>
+      <c r="K111" s="3"/>
+      <c r="L111" s="3"/>
+    </row>
+    <row r="112" spans="1:12">
+      <c r="G112" s="2"/>
+      <c r="I112" s="3"/>
+      <c r="J112" s="91"/>
+      <c r="K112" s="3"/>
+      <c r="L112" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3964,9 +4935,9 @@
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A72:A73"/>
   </mergeCells>
-  <conditionalFormatting sqref="C44">
+  <conditionalFormatting sqref="C45">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3978,7 +4949,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
+  <conditionalFormatting sqref="C56">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3990,7 +4961,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
+  <conditionalFormatting sqref="C51">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4002,7 +4973,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
+  <conditionalFormatting sqref="C46">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4014,7 +4985,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C52">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4026,7 +4997,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4038,7 +5009,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
+  <conditionalFormatting sqref="C47">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4050,7 +5021,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C39">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4062,37 +5033,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="formula" val="IF($C$34&gt;1,0.1,$O$42)"/>
-        <color rgb="FF00FF01"/>
-        <color rgb="FFFF7F82"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="formula" val="IF($C$25&gt;$C$35,0.1,$O$42)"/>
-        <color rgb="FF00FF01"/>
-        <color rgb="FFFF7F82"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="num" val="-2"/>
-        <cfvo type="formula" val="IF($O$39&gt;$C$32,-1,$O$42)"/>
-        <color rgb="FF00FF01"/>
-        <color rgb="FFFF7F82"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
+  <conditionalFormatting sqref="C65">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -4104,7 +5045,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
+  <conditionalFormatting sqref="C67">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="1"/>
@@ -4116,7 +5057,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
+  <conditionalFormatting sqref="C74">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4128,7 +5069,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
+  <conditionalFormatting sqref="C58">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0.95"/>
@@ -4138,7 +5079,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
+  <conditionalFormatting sqref="C32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4148,7 +5089,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
+  <conditionalFormatting sqref="C30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -4158,30 +5099,63 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="8">
+  <conditionalFormatting sqref="C35">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="formula" val="IF($C$35&gt;1,0.1,$O$49)"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFF7F82"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="formula" val="IF($C$25&gt;$C$36,0.1,$O$49)"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFF7F82"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="num" val="-2"/>
+        <cfvo type="formula" val="IF($O$41&gt;$C$33,-1,$O$49)"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFF7F82"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="9">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{5DA3BF6A-F4AE-C741-BD81-2AE26555EC93}">
       <formula1>$L$9:$L$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{A41A0E69-F7D3-A741-BD9A-54470CF0BDFA}">
-      <formula1>$L$11:$L$12</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{2B4F3B99-A92F-0243-A82E-385C2FB88239}">
-      <formula1>$L$13:$L$14</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C14 C19:C21 C23:C25" xr:uid="{30F53BB1-F524-6B4F-A972-7F8FA729E014}">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26" xr:uid="{4C29BBFC-90F4-9743-99F0-9EBD13C295AD}">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{A41A0E69-F7D3-A741-BD9A-54470CF0BDFA}">
+      <formula1>$L$12:$L$14</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{2B4F3B99-A92F-0243-A82E-385C2FB88239}">
+      <formula1>$L$16:$L$17</formula1>
+    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{43A4C1FF-ABA3-5C44-8A75-FC0862D518A3}">
-      <formula1>$L$15:$L$17</formula1>
+      <formula1>$L$19:$L$21</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{9E119CFB-DE75-D34D-852D-A0EED83568C6}">
+      <formula1>$L$23:$L$24</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{80DA8438-8DCA-D24F-A57D-2B18243B5230}">
-      <formula1>$L$21</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{9E119CFB-DE75-D34D-852D-A0EED83568C6}">
-      <formula1>$L$18:$L$19</formula1>
+      <formula1>$L$27</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C22" xr:uid="{BB74DD9C-C427-C847-911F-293B3DDC22E3}">
-      <formula1>$L$23:$L$25</formula1>
+      <formula1>$L$30:$L$33</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixes to settings spreadsheet.
</commit_message>
<xml_diff>
--- a/tools/CoMet_Settings_Tool.xlsx
+++ b/tools/CoMet_Settings_Tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjd/Desktop/DESKTOP_FILES/Genomics/genomics_gpu/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjd/genomics/genomics_gpu/tools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD2E289-BA58-834C-85CB-DE550A2C77A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA145AA7-05E3-A14D-B431-5F1DF09FCEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14640" yWindow="600" windowWidth="33640" windowHeight="30340" xr2:uid="{FA80413B-B473-9946-BFAA-BCC79B485766}"/>
+    <workbookView xWindow="5380" yWindow="1200" windowWidth="32620" windowHeight="37060" xr2:uid="{FA80413B-B473-9946-BFAA-BCC79B485766}"/>
   </bookViews>
   <sheets>
     <sheet name="CoMet_Settings_Tool" sheetId="6" r:id="rId1"/>
@@ -37,6 +37,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Wayne Joubert</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
     <comment ref="C13" authorId="0" shapeId="0" xr:uid="{7355445C-FEEA-3148-95F3-AF9E88314C96}">
@@ -113,6 +114,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="C17" authorId="1" shapeId="0" xr:uid="{DCD6514A-4BA7-CD43-9900-53C54C58711B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>certain features like "shrink" require single</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C18" authorId="0" shapeId="0" xr:uid="{80EC322D-9191-2A4E-B0CF-1F359AE6A4D8}">
       <text>
         <r>
@@ -650,7 +664,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>NOTE: this entry should be set bssed on empirical timing data</t>
+          <t>NOTE: this entry should be set manually based on empirical timing data</t>
         </r>
       </text>
     </comment>
@@ -672,7 +686,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="182">
   <si>
     <t>QUANTITY</t>
   </si>
@@ -809,9 +823,6 @@
     <t>sizeof double</t>
   </si>
   <si>
-    <t>sizeof float_t (value)</t>
-  </si>
-  <si>
     <t>sizeof FP16</t>
   </si>
   <si>
@@ -824,24 +835,15 @@
     <t>bits per vector elt</t>
   </si>
   <si>
-    <t>contstants etc.</t>
-  </si>
-  <si>
     <t>sizeof uint64</t>
   </si>
   <si>
-    <t>bytes per S</t>
-  </si>
-  <si>
     <t>sizeof float2</t>
   </si>
   <si>
     <t>sizeof float3</t>
   </si>
   <si>
-    <t>bytes per C</t>
-  </si>
-  <si>
     <t>num vector local</t>
   </si>
   <si>
@@ -969,9 +971,6 @@
   </si>
   <si>
     <t>comparisons/sec limit X 1e15</t>
-  </si>
-  <si>
-    <t>actual</t>
   </si>
   <si>
     <t>solver
@@ -1026,9 +1025,6 @@
     <t>fraction of avg allocation</t>
   </si>
   <si>
-    <t>stf006</t>
-  </si>
-  <si>
     <t>exec cmds</t>
   </si>
   <si>
@@ -1064,9 +1060,6 @@
     <t>GM_TALLY1_MAX_VALUE_BITS</t>
   </si>
   <si>
-    <t>. . . power 2</t>
-  </si>
-  <si>
     <t>machine epsilon</t>
   </si>
   <si>
@@ -1106,9 +1099,6 @@
     <t>is_duo</t>
   </si>
   <si>
-    <t>bytes per metric item</t>
-  </si>
-  <si>
     <t>is_shrink -- FIX</t>
   </si>
   <si>
@@ -1130,9 +1120,6 @@
     <t>TOTAL GPU</t>
   </si>
   <si>
-    <t>MEMORY:</t>
-  </si>
-  <si>
     <t>ComputeMetrics3WayBlock::ComputeMetrics3WayBlock</t>
   </si>
   <si>
@@ -1166,24 +1153,9 @@
     <t>is_threshold_tc -- FIX</t>
   </si>
   <si>
-    <t>num_metrics_local</t>
-  </si>
-  <si>
-    <t>metric items per metric</t>
-  </si>
-  <si>
-    <t>bytes per metric (elt)</t>
-  </si>
-  <si>
-    <t>bytes per metric (elt) 2-way</t>
-  </si>
-  <si>
     <t>bytes per metric index</t>
   </si>
   <si>
-    <t>bytes per metric (elt) + extras</t>
-  </si>
-  <si>
     <t>num_metrics_local 2-way</t>
   </si>
   <si>
@@ -1200,6 +1172,69 @@
   </si>
   <si>
     <t>ComputeMetrics2Way::ComputeMetrics2Way</t>
+  </si>
+  <si>
+    <t>constants etc.</t>
+  </si>
+  <si>
+    <t>bytes per metric</t>
+  </si>
+  <si>
+    <t>bytes per S (for denom)</t>
+  </si>
+  <si>
+    <t>bytes per C (for denom)</t>
+  </si>
+  <si>
+    <t>. . . power 2 (metric size limit)</t>
+  </si>
+  <si>
+    <t>(table) entries per metric</t>
+  </si>
+  <si>
+    <t>(metric)  items per metric</t>
+  </si>
+  <si>
+    <t>bytes per metric, 2-way case</t>
+  </si>
+  <si>
+    <t>bytes per metric+index+S+C</t>
+  </si>
+  <si>
+    <t>num_metrics_local (unshrunk)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>MEMORY USAGE CALCULATIONS:</t>
+  </si>
+  <si>
+    <t>GPU compute capability</t>
+  </si>
+  <si>
+    <t>ACTUAL</t>
+  </si>
+  <si>
+    <t>(table) entries per (metric) item</t>
+  </si>
+  <si>
+    <t>num_metric_items_local (unshrunk)</t>
+  </si>
+  <si>
+    <t>bytes needed per (metric) item</t>
+  </si>
+  <si>
+    <t>SUPPORTING CALCULATIONS:</t>
+  </si>
+  <si>
+    <t>num_metric_items_local_allocated</t>
+  </si>
+  <si>
+    <t>sizeof float_t (value) (GMFloat)</t>
+  </si>
+  <si>
+    <t>DEFUNCT</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1247,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1271,6 +1306,25 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1298,7 +1352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1411,51 +1465,6 @@
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1493,19 +1502,6 @@
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1846,11 +1842,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1894,46 +1927,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1942,16 +1963,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1963,16 +1984,16 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2023,22 +2044,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2050,73 +2071,70 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2132,31 +2150,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2164,6 +2182,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2646,7 +2709,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87649693-509E-D84D-8D62-271E15A24091}">
-  <dimension ref="A1:AC112"/>
+  <dimension ref="A1:AC115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -2665,8 +2728,8 @@
     <col min="11" max="11" width="15.83203125" style="2" customWidth="1"/>
     <col min="12" max="12" width="15" style="2" customWidth="1"/>
     <col min="13" max="13" width="1.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="27.5" style="53" customWidth="1"/>
-    <col min="15" max="15" width="14.1640625" style="53" customWidth="1"/>
+    <col min="14" max="14" width="27.5" style="49" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" style="49" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" style="1"/>
     <col min="17" max="17" width="5.1640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="3" style="1" customWidth="1"/>
@@ -2675,151 +2738,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="B1" s="30"/>
-      <c r="C1" s="36"/>
-      <c r="Q1" s="2">
-        <v>1</v>
-      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="32"/>
+      <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="10"/>
-      <c r="B2" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="62" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="30">
-        <f>Q1+1</f>
-        <v>2</v>
-      </c>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
+      <c r="B2" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="58" t="str">
+        <f>IF(C16=L21,"m1759_g","stf006")</f>
+        <v>m1759_g</v>
+      </c>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60"/>
+      <c r="AC2" s="60"/>
     </row>
     <row r="3" spans="1:29">
-      <c r="A3" s="95" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="67" t="str">
-        <f>IF(C$16=L$20,CONCATENATE("bsub -P ",C2," -nnodes ",C56," -W 10 -Is $SHELL"),"")</f>
-        <v/>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="30">
-        <f t="shared" ref="Q3:Q66" si="0">Q2+1</f>
-        <v>3</v>
-      </c>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
-      <c r="V3" s="69"/>
-      <c r="W3" s="69"/>
-      <c r="X3" s="69"/>
-      <c r="Y3" s="69"/>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="69"/>
-      <c r="AB3" s="69"/>
-      <c r="AC3" s="69"/>
+      <c r="A3" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="63" t="str">
+        <f>IF(C$16=L$20,CONCATENATE("bsub -P ",C2," -nnodes ",C56," -W 10 -Is $SHELL"),IF(C16=L21,CONCATENATE("salloc --account ",C2," --nodes ",C56," --qos early_science --time 1:00:00 --constraint gpu --gpus-per-node 4 --exclusive"),""))</f>
+        <v>salloc --account m1759_g --nodes 1479 --qos early_science --time 1:00:00 --constraint gpu --gpus-per-node 4 --exclusive</v>
+      </c>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65"/>
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
     </row>
     <row r="4" spans="1:29">
-      <c r="A4" s="96"/>
-      <c r="B4" s="72" t="str">
-        <f>IF(C$16=L$20,"executable=install_single_release_summit/bin/genomics_metric ar_opts='PAMI_IBV_ENABLE_DCT=1 PAMI_ENABLE_STRIPING=1 PAMI_IBV_ADAPTER_AFFINITY=0 PAMI_IBV_QP_SERVICE_LEVEL=8 PAMI_IBV_ENABLE_OOO_AR=1'","")</f>
-        <v/>
-      </c>
-      <c r="Q4" s="30">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
+      <c r="A4" s="91"/>
+      <c r="B4" s="68" t="str">
+        <f>IF(C$16=L$20,"executable=install_single_release_summit/bin/genomics_metric ar_opts='PAMI_IBV_ENABLE_DCT=1 PAMI_ENABLE_STRIPING=1 PAMI_IBV_ADAPTER_AFFINITY=0 PAMI_IBV_QP_SERVICE_LEVEL=8 PAMI_IBV_ENABLE_OOO_AR=1'",IF(C16=L21,"executable=install_single_release_perlmutter/bin/genomics_metric",""))</f>
+        <v>executable=install_single_release_perlmutter/bin/genomics_metric</v>
+      </c>
+      <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:29">
-      <c r="A5" s="96"/>
-      <c r="B5" s="72" t="str">
-        <f>IF(C$16=L$20,CONCATENATE("launch_command=""env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs ",C55," --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"""),"")</f>
-        <v/>
-      </c>
-      <c r="Q5" s="30">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
+      <c r="A5" s="91"/>
+      <c r="B5" s="68" t="str">
+        <f>IF(C$16=L$20,CONCATENATE("launch_command=""env OMP_NUM_THREADS=7 $ar_opts jsrun --nrs ",C55," --bind packed:7 --cpu_per_rs 7 --gpu_per_rs 1 --rs_per_host 6 --tasks_per_rs 1 -X 1"""),IF(C16=L21,"launch_command=""env OMP_PROC_BIND=spread OMP_PLACES=sockets OMP_NUM_THREADS=16 srun -n 4 -c 16 -G 4 --gpus-per-task=1 --gpu-bind=single:1""",""))</f>
+        <v>launch_command="env OMP_PROC_BIND=spread OMP_PLACES=sockets OMP_NUM_THREADS=16 srun -n 4 -c 16 -G 4 --gpus-per-task=1 --gpu-bind=single:1"</v>
+      </c>
+      <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:29">
-      <c r="A6" s="97"/>
-      <c r="B6" s="73" t="str">
-        <f>IF(C$16=L$20,CONCATENATE("$launch_command $executable --num_way ",C10," --metric_type ",C11," --sparse ",C12," --num_vector ",C13," --num_field ",C14," --all2all yes --compute_method GPU --num_proc_vector ",C19," --num_proc_field ",C20," --num_proc_repl ",C21," --tc ",O41," --num_tc_steps ",C23," --num_phase ",C24," --num_stage ",C25," --verbosity 1 --checksum no --phase_min ",MAX(0,C24-1)," --phase_max ",C24-1," --stage_min ",MAX(0,C25-1)," --stage_max ",C25-1),"")</f>
-        <v/>
-      </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="76"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="30">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R6" s="75"/>
-      <c r="S6" s="75"/>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="75"/>
-      <c r="W6" s="75"/>
-      <c r="X6" s="75"/>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="75"/>
-      <c r="AA6" s="75"/>
-      <c r="AB6" s="75"/>
-      <c r="AC6" s="75"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="69" t="str">
+        <f>CONCATENATE("$launch_command $executable --num_way ",C10," --metric_type ",C11," --sparse ",C12," --num_vector ",C13," --num_field ",C14," --all2all yes --compute_method GPU --num_proc_vector ",C19," --num_proc_field ",C20," --num_proc_repl ",C21," --tc ",O41," --num_tc_steps ",C23," --num_phase ",C24," --num_stage ",C25," --verbosity 1 --checksum no --phase_min ",MAX(0,C24-1)," --phase_max ",C24-1," --stage_min ",MAX(0,C25-1)," --stage_max ",C25-1)</f>
+        <v>$launch_command $executable --num_way 3 --metric_type duo --sparse yes --num_vector 672768 --num_field 1008000 --all2all yes --compute_method GPU --num_proc_vector 73 --num_proc_field 1 --num_proc_repl 81 --tc 2 --num_tc_steps 2 --num_phase 1 --num_stage 64 --verbosity 1 --checksum no --phase_min 0 --phase_max 0 --stage_min 63 --stage_max 63</v>
+      </c>
+      <c r="C6" s="70"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="71"/>
+      <c r="U6" s="71"/>
+      <c r="V6" s="71"/>
+      <c r="W6" s="71"/>
+      <c r="X6" s="71"/>
+      <c r="Y6" s="71"/>
+      <c r="Z6" s="71"/>
+      <c r="AA6" s="71"/>
+      <c r="AB6" s="71"/>
+      <c r="AC6" s="71"/>
     </row>
     <row r="7" spans="1:29">
       <c r="B7" s="13"/>
-      <c r="C7" s="37"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
@@ -2830,11 +2877,11 @@
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="12"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
       <c r="P7" s="12"/>
-      <c r="Q7" s="30">
-        <f t="shared" si="0"/>
+      <c r="Q7" s="26">
+        <f>7</f>
         <v>7</v>
       </c>
       <c r="R7" s="12"/>
@@ -2859,11 +2906,11 @@
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="98" t="s">
+      <c r="F8" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="99"/>
-      <c r="H8" s="100"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="95"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="9" t="s">
@@ -2871,30 +2918,30 @@
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" s="54"/>
-      <c r="Q8" s="30">
-        <f t="shared" si="0"/>
+      <c r="N8" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="O8" s="50"/>
+      <c r="Q8" s="26">
+        <f t="shared" ref="Q8:Q66" si="0">Q7+1</f>
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:29">
-      <c r="B9" s="30"/>
-      <c r="C9" s="36"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="26" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="32"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" s="47" t="s">
-        <v>99</v>
+      <c r="H9" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>174</v>
       </c>
       <c r="K9" s="5" t="s">
         <v>6</v>
@@ -2902,45 +2949,45 @@
       <c r="L9" s="5">
         <v>2</v>
       </c>
-      <c r="N9" s="53" t="s">
+      <c r="N9" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="O9" s="55">
+      <c r="O9" s="51">
         <f>1024*1024*1024</f>
         <v>1073741824</v>
       </c>
-      <c r="Q9" s="30">
+      <c r="Q9" s="26">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:29">
-      <c r="A10" s="101" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="96" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="38">
-        <v>2</v>
-      </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="18" t="s">
+      <c r="C10" s="34">
+        <v>3</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="19">
         <f>6*0.85</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="20">
         <f>16*0.95</f>
         <v>15.2</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H10" s="21">
         <f>40*0.975</f>
         <v>39</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="44">
         <f>IF(C$16=F$9,F10,IF(C$16=G$9,G10,H10))</f>
         <v>39</v>
       </c>
@@ -2948,31 +2995,31 @@
       <c r="L10" s="5">
         <v>3</v>
       </c>
-      <c r="N10" s="53" t="s">
+      <c r="N10" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="55">
+      <c r="O10" s="51">
         <f>1000000000</f>
         <v>1000000000</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="Q10" s="26">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:29">
-      <c r="A11" s="102"/>
-      <c r="B11" s="32" t="s">
+      <c r="A11" s="97"/>
+      <c r="B11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="19" t="s">
+      <c r="C11" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="18">
         <v>1</v>
       </c>
       <c r="G11" s="2">
@@ -2981,28 +3028,28 @@
       <c r="H11" s="14">
         <v>4</v>
       </c>
-      <c r="I11" s="49">
+      <c r="I11" s="45">
         <f t="shared" ref="I11:I12" si="1">IF(C$16=F$9,F11,IF(C$16=G$9,G11,H11))</f>
         <v>4</v>
       </c>
-      <c r="Q11" s="30">
+      <c r="Q11" s="26">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="10"/>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="31"/>
+      <c r="E12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>31</v>
       </c>
       <c r="G12" s="2">
@@ -3012,7 +3059,7 @@
         <f>256*0.9</f>
         <v>230.4</v>
       </c>
-      <c r="I12" s="49">
+      <c r="I12" s="45">
         <f t="shared" si="1"/>
         <v>230.4</v>
       </c>
@@ -3022,39 +3069,39 @@
       <c r="L12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N12" s="53" t="s">
+      <c r="N12" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="O12" s="53">
+      <c r="O12" s="49">
         <v>8</v>
       </c>
-      <c r="Q12" s="30">
+      <c r="Q12" s="26">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="10"/>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="39">
-        <v>15360</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="20" t="s">
+      <c r="C13" s="35">
+        <v>672768</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="110" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="108">
         <v>18688</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="32">
         <v>4608</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="107">
         <v>1500</v>
       </c>
-      <c r="I13" s="49">
+      <c r="I13" s="45">
         <f>IF(C$16=F$9,F13,IF(C$16=G$9,G13,H13))</f>
         <v>1500</v>
       </c>
@@ -3062,459 +3109,454 @@
       <c r="L13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q13" s="30">
+      <c r="Q13" s="26">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="10"/>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="40">
-        <v>1048576</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="49"/>
+      <c r="C14" s="36">
+        <v>1008000</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="111" t="s">
+        <v>173</v>
+      </c>
+      <c r="F14" s="109">
+        <v>350</v>
+      </c>
+      <c r="G14" s="105">
+        <v>700</v>
+      </c>
+      <c r="H14" s="106">
+        <v>800</v>
+      </c>
+      <c r="I14" s="45">
+        <f>IF(C$16=F$9,F14,IF(C$16=G$9,G14,H14))</f>
+        <v>800</v>
+      </c>
       <c r="L14" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="N14" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="53">
+      <c r="O14" s="49">
         <v>4</v>
       </c>
-      <c r="Q14" s="30">
+      <c r="Q14" s="26">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:29">
-      <c r="B15" s="34"/>
-      <c r="C15" s="41"/>
-      <c r="E15" s="50" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="37"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
+      <c r="N15" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="O15" s="49">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="26">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="90" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F16" s="41">
         <f>F11*F13</f>
         <v>18688</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G16" s="41">
         <f>G11*G13</f>
         <v>27648</v>
       </c>
-      <c r="H15" s="45">
+      <c r="H16" s="41">
         <f>H11*H13</f>
         <v>6000</v>
       </c>
-      <c r="I15" s="49">
-        <f t="shared" ref="I15:I19" si="2">IF(C$16=F$9,F15,IF(C$16=G$9,G15,H15))</f>
+      <c r="I16" s="45">
+        <f>IF(C$16=F$9,F16,IF(C$16=G$9,G16,H16))</f>
         <v>6000</v>
       </c>
-      <c r="N15" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="O15" s="53">
-        <v>8</v>
-      </c>
-      <c r="Q15" s="30">
-        <f t="shared" si="0"/>
+      <c r="K16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="O16" s="49">
+        <f>IF(C17=L23,O14,O15)</f>
+        <v>4</v>
+      </c>
+      <c r="Q16" s="26">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="98"/>
+      <c r="B17" s="28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:29">
-      <c r="A16" s="95" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="50" t="s">
+      <c r="C17" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="25"/>
+      <c r="E17" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="45">
+      <c r="F17" s="41">
         <f>F10*$O9</f>
         <v>5476083302.3999996</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G17" s="41">
         <f>G10*$O9</f>
         <v>16320875724.799999</v>
       </c>
-      <c r="H16" s="45">
+      <c r="H17" s="41">
         <f>H10*$O9</f>
         <v>41875931136</v>
       </c>
-      <c r="I16" s="49">
-        <f t="shared" si="2"/>
+      <c r="I17" s="45">
+        <f>IF(C$16=F$9,F17,IF(C$16=G$9,G17,H17))</f>
         <v>41875931136</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="O16" s="53">
-        <f>IF(C17=L23,O14,O15)</f>
-        <v>4</v>
-      </c>
-      <c r="Q16" s="30">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="103"/>
-      <c r="B17" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="45">
-        <f>F12*$O9/F11</f>
-        <v>33285996544</v>
-      </c>
-      <c r="G17" s="45">
-        <f t="shared" ref="G17" si="3">G12*$O9/G11</f>
-        <v>75161927680</v>
-      </c>
-      <c r="H17" s="45">
-        <f t="shared" ref="H17" si="4">H12*$O9/H11</f>
-        <v>61847529062.400002</v>
-      </c>
-      <c r="I17" s="49">
-        <f t="shared" si="2"/>
-        <v>61847529062.400002</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q17" s="30">
+      <c r="Q17" s="26">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="10"/>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="I18" s="49"/>
-      <c r="N18" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="O18" s="53">
+      <c r="D18" s="25"/>
+      <c r="E18" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="41">
+        <f>F12*$O9/F11</f>
+        <v>33285996544</v>
+      </c>
+      <c r="G18" s="41">
+        <f>G12*$O9/G11</f>
+        <v>75161927680</v>
+      </c>
+      <c r="H18" s="41">
+        <f>H12*$O9/H11</f>
+        <v>61847529062.400002</v>
+      </c>
+      <c r="I18" s="45">
+        <f>IF(C$16=F$9,F18,IF(C$16=G$9,G18,H18))</f>
+        <v>61847529062.400002</v>
+      </c>
+      <c r="N18" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" s="49">
         <v>8</v>
       </c>
-      <c r="Q18" s="30">
+      <c r="Q18" s="26">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="10"/>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="35">
+        <v>73</v>
+      </c>
+      <c r="D19" s="25"/>
+      <c r="K19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q19" s="26">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="10"/>
+      <c r="B20" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="35">
         <v>1</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="D20" s="25"/>
+      <c r="E20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="3">
         <f>100000000/30</f>
         <v>3333333.3333333335</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G20" s="3">
         <v>300000</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="49">
-        <f t="shared" si="2"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="45">
+        <f>IF(C$16=F$9,F20,IF(C$16=G$9,G20,H20))</f>
         <v>0</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q19" s="30">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="10"/>
-      <c r="B20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="39">
-        <v>1</v>
-      </c>
-      <c r="D20" s="29"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N20" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="O20" s="53">
+      <c r="N20" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="49">
         <v>2</v>
       </c>
-      <c r="Q20" s="30">
+      <c r="Q20" s="26">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="10"/>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="39">
-        <v>1</v>
-      </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="2">
-        <f>IF(N38=1,F22,F26)</f>
-        <v>2.0579999999999998</v>
-      </c>
-      <c r="G21" s="2">
-        <f>IF($O$38=1,G22,G26)</f>
-        <v>295.63299999999998</v>
-      </c>
-      <c r="H21" s="2">
-        <f>IF($O$38=1,H22,H26)</f>
-        <v>1687.5</v>
-      </c>
-      <c r="I21" s="48">
-        <f t="shared" ref="I21:I23" si="5">IF(C$16=F$9,F21,IF(C$16=G$9,G21,H21))</f>
-        <v>1687.5</v>
-      </c>
+      <c r="C21" s="35">
+        <v>81</v>
+      </c>
+      <c r="D21" s="25"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="N21" s="53" t="s">
-        <v>47</v>
-      </c>
-      <c r="O21" s="53">
+        <v>127</v>
+      </c>
+      <c r="N21" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" s="49">
         <v>1</v>
       </c>
-      <c r="Q21" s="30">
+      <c r="Q21" s="26">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="10"/>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="39" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="29"/>
-      <c r="E22" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="6">
-        <f>IF(O38=1,F23,F24)</f>
-        <v>4.2889999999999997</v>
-      </c>
-      <c r="G22" s="6">
-        <f>IF($O$34=1,G23,IF($O$34=2,G24,G25))</f>
-        <v>295.63299999999998</v>
-      </c>
-      <c r="H22" s="6">
-        <f>IF($O$34=1,H23,IF($O$34=2,H24,H25))</f>
-        <v>1687.5</v>
-      </c>
-      <c r="I22" s="11">
-        <f t="shared" si="5"/>
-        <v>1687.5</v>
-      </c>
-      <c r="N22" s="53" t="s">
-        <v>139</v>
-      </c>
-      <c r="O22" s="53">
+      <c r="C22" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="2">
+        <f>IF(N38=1,F23,F27)</f>
+        <v>2.0579999999999998</v>
+      </c>
+      <c r="G22" s="2">
+        <f>IF($O$38=1,G23,G27)</f>
+        <v>132.9127</v>
+      </c>
+      <c r="H22" s="2">
+        <f>IF($O$38=1,H23,H27)</f>
+        <v>843.75</v>
+      </c>
+      <c r="I22" s="44">
+        <f>IF(C$16=F$9,F22,IF(C$16=G$9,G22,H22))</f>
+        <v>843.75</v>
+      </c>
+      <c r="N22" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="O22" s="49">
         <f>(1/O12)</f>
         <v>0.125</v>
       </c>
-      <c r="Q22" s="30">
+      <c r="Q22" s="26">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="10"/>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="39">
-        <v>4</v>
-      </c>
-      <c r="D23" s="29"/>
+      <c r="C23" s="35">
+        <v>2</v>
+      </c>
+      <c r="D23" s="25"/>
       <c r="E23" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F23" s="6">
+        <f>IF(O38=1,F24,F25)</f>
+        <v>9.1080000000000005</v>
+      </c>
+      <c r="G23" s="6">
+        <f>IF($O$34=1,G24,IF($O$34=2,G25,G26))</f>
+        <v>295.63299999999998</v>
+      </c>
+      <c r="H23" s="6">
+        <f>IF($O$34=1,H24,IF($O$34=2,H25,H26))</f>
+        <v>1687.5</v>
+      </c>
+      <c r="I23" s="11">
+        <f>IF(C$16=F$9,F23,IF(C$16=G$9,G23,H23))</f>
+        <v>1687.5</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N23" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="O23" s="49">
+        <f>IF(C22=L31,O20,IF(C22=L32,O21,IF(C22=L33,O22,0)))</f>
+        <v>0.125</v>
+      </c>
+      <c r="Q23" s="26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="10"/>
+      <c r="B24" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="35">
+        <v>1</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="6">
         <f>IF(C17=L23,4.289,1.697)</f>
         <v>4.2889999999999997</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G24" s="6">
         <f>IF($C$17=$L$23,94.768,29.586)</f>
         <v>94.768000000000001</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N23" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="O23" s="53">
-        <f>IF(C22=L31,O20,IF(C22=L32,O21,IF(C22=L33,O22,0)))</f>
-        <v>0.125</v>
-      </c>
-      <c r="Q23" s="30">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="10"/>
-      <c r="B24" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="39">
-        <v>1</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="6">
-        <f>9.108</f>
-        <v>9.1080000000000005</v>
-      </c>
-      <c r="G24" s="6">
-        <f>IF($O$37=1,295.633,IF($O$33=1,71.587,104.37))</f>
-        <v>295.63299999999998</v>
-      </c>
       <c r="H24" s="6"/>
       <c r="I24" s="11">
-        <f t="shared" ref="I24:I29" si="6">IF(C$16=F$9,F24,IF(C$16=G$9,G24,H24))</f>
+        <f>IF(C$16=F$9,F24,IF(C$16=G$9,G24,H24))</f>
         <v>0</v>
       </c>
       <c r="K24" s="5"/>
       <c r="L24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="Q24" s="30">
+      <c r="Q24" s="26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="10"/>
-      <c r="B25" s="85" t="s">
+      <c r="B25" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="86">
-        <v>1</v>
-      </c>
-      <c r="D25" s="29"/>
+      <c r="C25" s="82">
+        <v>64</v>
+      </c>
+      <c r="D25" s="25"/>
       <c r="E25" s="4" t="s">
-        <v>140</v>
+        <v>89</v>
+      </c>
+      <c r="F25" s="6">
+        <f>9.108</f>
+        <v>9.1080000000000005</v>
       </c>
       <c r="G25" s="6">
         <f>IF($O$37=1,295.633,IF($O$33=1,71.587,104.37))</f>
         <v>295.63299999999998</v>
       </c>
-      <c r="H25" s="6">
-        <v>1687.5</v>
-      </c>
+      <c r="H25" s="6"/>
       <c r="I25" s="11">
-        <f t="shared" si="6"/>
-        <v>1687.5</v>
-      </c>
-      <c r="N25" s="53" t="s">
-        <v>53</v>
-      </c>
-      <c r="O25" s="53">
+        <f>IF(C$16=F$9,F25,IF(C$16=G$9,G25,H25))</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="O25" s="49">
         <f>O15</f>
         <v>8</v>
       </c>
-      <c r="Q25" s="30">
+      <c r="Q25" s="26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="10"/>
-      <c r="B26" s="87" t="s">
-        <v>138</v>
-      </c>
-      <c r="C26" s="88">
-        <v>1000</v>
-      </c>
-      <c r="D26" s="29"/>
+      <c r="B26" s="83" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="84">
+        <v>400</v>
+      </c>
+      <c r="D26" s="25"/>
       <c r="E26" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="6">
-        <f>IF(O34=1,F27,F28)</f>
-        <v>2.0579999999999998</v>
+        <v>133</v>
       </c>
       <c r="G26" s="6">
-        <f>IF($O$34=1,G27,IF($O$35=1,G28,G29))</f>
-        <v>132.9127</v>
+        <f>IF($O$37=1,295.633,IF($O$33=1,71.587,104.37))</f>
+        <v>295.63299999999998</v>
       </c>
       <c r="H26" s="6">
-        <f>IF($O$34=1,H27,IF($O$35=1,H28,H29))</f>
-        <v>843.75</v>
+        <v>1687.5</v>
       </c>
       <c r="I26" s="11">
-        <f t="shared" si="6"/>
-        <v>843.75</v>
+        <f>IF(C$16=F$9,F26,IF(C$16=G$9,G26,H26))</f>
+        <v>1687.5</v>
       </c>
       <c r="K26" s="5" t="s">
         <v>7</v>
@@ -3522,1412 +3564,1469 @@
       <c r="L26" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N26" s="53" t="s">
-        <v>54</v>
-      </c>
-      <c r="O26" s="53">
+      <c r="N26" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="O26" s="49">
         <f>2*O15</f>
         <v>16</v>
       </c>
-      <c r="Q26" s="30">
+      <c r="Q26" s="26">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:17">
-      <c r="B27" s="34"/>
-      <c r="C27" s="41"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="37"/>
       <c r="E27" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F27" s="6">
-        <f>IF(C17=L23,5.695,2.445)</f>
-        <v>5.6950000000000003</v>
+        <f>IF(O34=1,F28,F29)</f>
+        <v>2.0579999999999998</v>
       </c>
       <c r="G27" s="6">
-        <f>IF($C$17=$L$23,72.499,27.755)</f>
-        <v>72.498999999999995</v>
-      </c>
-      <c r="H27" s="6"/>
+        <f>IF($O$34=1,G28,IF($O$35=1,G29,G30))</f>
+        <v>132.9127</v>
+      </c>
+      <c r="H27" s="6">
+        <f>IF($O$34=1,H28,IF($O$35=1,H29,H30))</f>
+        <v>843.75</v>
+      </c>
       <c r="I27" s="11">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>IF(C$16=F$9,F27,IF(C$16=G$9,G27,H27))</f>
+        <v>843.75</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="O27" s="53">
+      <c r="N27" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="O27" s="49">
         <f>IF(C10=L9,O25,O26)</f>
-        <v>8</v>
-      </c>
-      <c r="Q27" s="30">
+        <v>16</v>
+      </c>
+      <c r="Q27" s="26">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" s="10"/>
-      <c r="B28" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="83">
+      <c r="B28" s="80" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="79">
         <v>0.1</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F28" s="6">
-        <f>2.058</f>
-        <v>2.0579999999999998</v>
+        <f>IF(C17=L23,5.695,2.445)</f>
+        <v>5.6950000000000003</v>
       </c>
       <c r="G28" s="6">
-        <f>IF($O$37=1,132.9127,IF($O$33=1,21.163,23.672))</f>
-        <v>132.9127</v>
+        <f>IF($C$17=$L$23,72.499,27.755)</f>
+        <v>72.498999999999995</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="11">
-        <f t="shared" si="6"/>
+        <f>IF(C$16=F$9,F28,IF(C$16=G$9,G28,H28))</f>
         <v>0</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q28" s="30">
+      <c r="Q28" s="26">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="B29" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="80">
-        <f>O62*10*C14</f>
-        <v>0.62495129599999999</v>
+        <v>126</v>
+      </c>
+      <c r="C29" s="76">
+        <f>O63*10*C14</f>
+        <v>0.60076799999999997</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>141</v>
+        <v>91</v>
+      </c>
+      <c r="F29" s="6">
+        <f>2.058</f>
+        <v>2.0579999999999998</v>
       </c>
       <c r="G29" s="6">
         <f>IF($O$37=1,132.9127,IF($O$33=1,21.163,23.672))</f>
         <v>132.9127</v>
       </c>
-      <c r="H29" s="6">
-        <v>843.75</v>
-      </c>
+      <c r="H29" s="6"/>
       <c r="I29" s="11">
-        <f t="shared" si="6"/>
-        <v>843.75</v>
-      </c>
-      <c r="N29" s="53" t="s">
-        <v>105</v>
-      </c>
-      <c r="O29" s="53">
+        <f>IF(C$16=F$9,F29,IF(C$16=G$9,G29,H29))</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="O29" s="49">
         <f>IF(C11=L12,O16,IF(O37=1,O23,2*O15))</f>
         <v>0.125</v>
       </c>
-      <c r="Q29" s="30">
+      <c r="Q29" s="26">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="B30" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="42">
+        <v>125</v>
+      </c>
+      <c r="C30" s="38">
         <f>C29/C28</f>
-        <v>6.2495129599999997</v>
+        <v>6.0076799999999997</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" s="6">
+        <f>IF($O$37=1,132.9127,IF($O$33=1,21.163,23.672))</f>
+        <v>132.9127</v>
+      </c>
+      <c r="H30" s="6">
+        <v>843.75</v>
+      </c>
+      <c r="I30" s="11">
+        <f>IF(C$16=F$9,F30,IF(C$16=G$9,G30,H30))</f>
+        <v>843.75</v>
       </c>
       <c r="K30" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L30" s="53" t="s">
+      <c r="L30" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="N30" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="O30" s="53">
+      <c r="N30" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="O30" s="49">
         <f>IF(C11=L12,O16,IF(O37=1,4,2*O15))</f>
         <v>4</v>
       </c>
-      <c r="Q30" s="30">
+      <c r="Q30" s="26">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="B31" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C31" s="3">
-        <f>CEILING(O60,POWER(2,O40))/POWER(2,O40)-1</f>
-        <v>16777215</v>
+        <f>CEILING(O61,POWER(2,O40))/POWER(2,O40)-1</f>
+        <v>8388607</v>
       </c>
       <c r="K31" s="5"/>
-      <c r="L31" s="53" t="s">
+      <c r="L31" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="Q31" s="30">
+      <c r="Q31" s="26">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="B32" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="82">
+        <v>125</v>
+      </c>
+      <c r="C32" s="78">
         <f>C14/C31</f>
-        <v>6.2500003725290521E-2</v>
+        <v>0.12016297819173076</v>
       </c>
       <c r="K32" s="5"/>
-      <c r="L32" s="53" t="s">
+      <c r="L32" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="N32" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="O32" s="53">
+      <c r="N32" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="O32" s="49">
         <f>IF(C20&gt;1,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q32" s="30">
+      <c r="Q32" s="26">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
     </row>
     <row r="33" spans="2:17">
       <c r="B33" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C33" s="2">
         <f>IF(C16=L19,0,O42)</f>
         <v>5</v>
       </c>
       <c r="K33" s="6"/>
-      <c r="L33" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="N33" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="O33" s="53">
+      <c r="L33" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="N33" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="O33" s="49">
         <f>IF(C12=L17,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q33" s="30">
+      <c r="Q33" s="26">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:17">
-      <c r="B34" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="45">
+      <c r="B34" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="41">
         <f>IF(O38=1,1+FLOOR(C19,2)/2,(C19+1)*(C19+2)/2)</f>
-        <v>1</v>
-      </c>
-      <c r="L34" s="53" t="s">
-        <v>137</v>
-      </c>
-      <c r="N34" s="53" t="s">
-        <v>81</v>
-      </c>
-      <c r="O34" s="53">
+        <v>2775</v>
+      </c>
+      <c r="L34" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="N34" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="O34" s="49">
         <f>IF(C11=L12,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q34" s="30">
+      <c r="Q34" s="26">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:17">
       <c r="B35" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="42">
+        <v>125</v>
+      </c>
+      <c r="C35" s="38">
         <f>C24/C34</f>
-        <v>1</v>
-      </c>
-      <c r="L35" s="53"/>
-      <c r="N35" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="O35" s="53">
+        <v>3.6036036036036037E-4</v>
+      </c>
+      <c r="L35" s="49"/>
+      <c r="N35" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="O35" s="49">
         <f>IF(C11=L13,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Q35" s="30">
+      <c r="Q35" s="26">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="2:17">
-      <c r="B36" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" s="44">
+      <c r="B36" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="40">
         <f>IF(O38=1,1,O49)</f>
-        <v>1</v>
-      </c>
-      <c r="L36" s="53"/>
-      <c r="N36" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="O36" s="53">
+        <v>1E+30</v>
+      </c>
+      <c r="L36" s="49"/>
+      <c r="N36" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="O36" s="49">
         <f>IF(C11=L14,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q36" s="30">
+      <c r="Q36" s="26">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="2:17">
       <c r="B37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="42">
+        <v>125</v>
+      </c>
+      <c r="C37" s="38">
         <f>C25/C36</f>
+        <v>6.3999999999999994E-29</v>
+      </c>
+      <c r="L37" s="49"/>
+      <c r="N37" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="O37" s="49">
+        <f>IF(AND(C22=L30,O34=0),0,1)</f>
         <v>1</v>
       </c>
-      <c r="L37" s="53"/>
-      <c r="N37" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="O37" s="53">
-        <f>IF(C22=L30,0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="Q37" s="30">
+      <c r="Q37" s="26">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
     </row>
     <row r="38" spans="2:17">
       <c r="B38" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="60">
+        <v>98</v>
+      </c>
+      <c r="C38" s="56">
         <f>IF(O38=1,(1+FLOOR(C19,2)/2)/C21/C24,(C19+1)*(C19+2)/C21/C24)</f>
-        <v>1</v>
-      </c>
-      <c r="L38" s="53"/>
-      <c r="N38" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="O38" s="55">
+        <v>68.518518518518519</v>
+      </c>
+      <c r="L38" s="49"/>
+      <c r="N38" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="O38" s="51">
         <f>IF(C10=L9,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Q38" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="26">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:17">
       <c r="B39" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="42">
+        <v>99</v>
+      </c>
+      <c r="C39" s="38">
         <f>(CEILING(C38,1)-C38)/C38</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="53"/>
-      <c r="N39" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="O39" s="55">
+        <v>7.0270270270270194E-3</v>
+      </c>
+      <c r="L39" s="49"/>
+      <c r="N39" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="O39" s="51">
         <f>IF(C10=L10,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q39" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="26">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:17">
       <c r="B40" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="60" t="str">
+        <v>114</v>
+      </c>
+      <c r="C40" s="56">
         <f>IF(O39=1,C78/6/C25,"N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="N40" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="N40" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="O40" s="53">
+      <c r="O40" s="49">
         <f>O38*2+O39*3</f>
-        <v>2</v>
-      </c>
-      <c r="Q40" s="30">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="26">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
     </row>
     <row r="41" spans="2:17">
-      <c r="N41" s="53" t="s">
+      <c r="N41" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="O41" s="53">
+      <c r="O41" s="49">
         <f>IF(C22=L30,0,IF(C22=L31,1,2))</f>
         <v>2</v>
       </c>
-      <c r="Q41" s="30">
+      <c r="Q41" s="26">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
     </row>
     <row r="42" spans="2:17">
       <c r="B42" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C42" s="3">
         <f>O37*2*(CEILING(C79,C23)/C23)*(2*C77)*O23</f>
-        <v>2013265920</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="N42" s="53" t="s">
-        <v>102</v>
-      </c>
-      <c r="O42" s="53">
+        <v>2322432000</v>
+      </c>
+      <c r="N42" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="O42" s="49">
         <v>5</v>
       </c>
-      <c r="Q42" s="30">
+      <c r="Q42" s="26">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
     </row>
     <row r="43" spans="2:17">
       <c r="B43" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="3">
-        <f>IF(O38=1,L99+L100+L101+L102+L103,"N/A")</f>
-        <v>32967536640</v>
-      </c>
-      <c r="E43" s="2">
-        <f>IF(O38=1,3*C82+(2+O32)*C83+C42+IF(O43=1,C77*C77*4*(4+8),0),"N/A")</f>
-        <v>32967229440</v>
-      </c>
-      <c r="N43" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="O43" s="53">
+        <v>57</v>
+      </c>
+      <c r="C43" s="3" t="str">
+        <f>IF(O38=1,L108,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="N43" s="49" t="s">
+        <v>136</v>
+      </c>
+      <c r="O43" s="49">
         <f>O37</f>
         <v>1</v>
       </c>
-      <c r="Q43" s="30">
+      <c r="Q43" s="26">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
     </row>
     <row r="44" spans="2:17">
       <c r="B44" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="3" t="str">
-        <f>IF(O39=1,L97+L98+L99+L100,"N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="E44" s="2" t="str">
-        <f>IF(O39=1,(3*C82)+(2*C82+2*C83+O32*2*C83+O34*3*C83)+C42+IF(O43=1,C77*C77*4*(4+8)-2*C82,0), "N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="N44" s="53" t="s">
-        <v>154</v>
-      </c>
-      <c r="O44" s="53">
+        <v>59</v>
+      </c>
+      <c r="C44" s="3">
+        <f>IF(O39=1,L108,"N/A")</f>
+        <v>16085225664</v>
+      </c>
+      <c r="N44" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="O44" s="49">
         <v>1</v>
       </c>
-      <c r="Q44" s="30">
+      <c r="Q44" s="26">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
     </row>
     <row r="45" spans="2:17">
       <c r="B45" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C45" s="3">
         <f>IF(O38=1,C43,C44)</f>
-        <v>32967536640</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="N45" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="O45" s="53">
+        <v>16085225664</v>
+      </c>
+      <c r="N45" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="O45" s="49">
         <v>1</v>
       </c>
-      <c r="Q45" s="30">
+      <c r="Q45" s="26">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
     <row r="46" spans="2:17">
       <c r="B46" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C46" s="42">
-        <f>C45/I16</f>
-        <v>0.78726695134089542</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="N46" s="53" t="s">
-        <v>161</v>
-      </c>
-      <c r="O46" s="53">
-        <f>IF(C22=L33,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Q46" s="30">
+        <v>70</v>
+      </c>
+      <c r="C46" s="38">
+        <f>C45/I17</f>
+        <v>0.38411625073506284</v>
+      </c>
+      <c r="N46" s="49" t="s">
+        <v>152</v>
+      </c>
+      <c r="O46" s="49">
+        <f>IF(AND(C22=L33, I14=750),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="26">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="2:17">
       <c r="B47" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="42">
-        <f>C45/I16</f>
-        <v>0.78726695134089542</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="N47" s="53" t="s">
-        <v>162</v>
-      </c>
-      <c r="O47" s="53">
+        <v>119</v>
+      </c>
+      <c r="C47" s="38">
+        <f>C45/I17</f>
+        <v>0.38411625073506284</v>
+      </c>
+      <c r="N47" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="O47" s="49">
+        <f>IF(AND(O37=1,C17="single"),1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q47" s="30">
+      <c r="Q47" s="26">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
     </row>
     <row r="48" spans="2:17">
-      <c r="E48" s="2"/>
-      <c r="Q48" s="30">
+      <c r="Q48" s="26">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
     </row>
     <row r="49" spans="2:17">
       <c r="B49" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" s="3">
-        <f>IF(O38=1,K99+K100+K101+K102+K103,"N/A")</f>
-        <v>34999554048</v>
-      </c>
-      <c r="E49" s="2">
-        <f>IF(O38=1,C82+(C43-C42)+2*C86+C89+IF(O43=1,C77*C77*C494*(4+8),0),"N/A")</f>
-        <v>34984700313.599998</v>
-      </c>
-      <c r="N49" s="53" t="s">
-        <v>89</v>
-      </c>
-      <c r="O49" s="56">
+        <v>62</v>
+      </c>
+      <c r="C49" s="3" t="str">
+        <f>IF(O38=1,K108,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="N49" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="O49" s="52">
         <v>1E+30</v>
       </c>
-      <c r="Q49" s="30">
+      <c r="Q49" s="26">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
     </row>
     <row r="50" spans="2:17">
       <c r="B50" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="3" t="str">
-        <f>IF(O39=1,K97+K98+K99+K101+K102,"N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="E50" s="2" t="str">
-        <f>IF(O39=1,C82+(C44-C42)+3*C86+C89+4*C82,"N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="Q50" s="30">
+        <v>63</v>
+      </c>
+      <c r="C50" s="3">
+        <f>IF(O39=1,K108,"N/A")</f>
+        <v>59131383344.639999</v>
+      </c>
+      <c r="Q50" s="26">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
     <row r="51" spans="2:17">
       <c r="B51" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C51" s="3">
         <f>IF(O38=1,C49,C50)</f>
-        <v>34999554048</v>
-      </c>
-      <c r="D51" s="29"/>
-      <c r="E51" s="2"/>
-      <c r="N51" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="O51" s="55">
+        <v>59131383344.639999</v>
+      </c>
+      <c r="D51" s="25"/>
+      <c r="N51" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="O51" s="51">
         <f>IF(O34=1,O12*O16,2)</f>
         <v>2</v>
       </c>
-      <c r="Q51" s="30">
+      <c r="Q51" s="26">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
     </row>
     <row r="52" spans="2:17">
       <c r="B52" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="42">
-        <f>C51/I17</f>
-        <v>0.5659006039301554</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="N52" s="53" t="s">
-        <v>165</v>
-      </c>
-      <c r="O52" s="55">
-        <f>IF(O34=1,O16,POWER(2,O40)*O15/2)</f>
-        <v>16</v>
-      </c>
-      <c r="Q52" s="30">
+        <v>71</v>
+      </c>
+      <c r="C52" s="38">
+        <f>C51/I18</f>
+        <v>0.95608319751918314</v>
+      </c>
+      <c r="N52" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="O52" s="49">
+        <f>IF(O34=1,1,POWER(2,O40))</f>
+        <v>8</v>
+      </c>
+      <c r="Q52" s="26">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
     <row r="53" spans="2:17">
-      <c r="N53" s="53" t="s">
-        <v>166</v>
-      </c>
-      <c r="O53" s="53">
+      <c r="N53" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="O53" s="51">
+        <f>O52*O16</f>
+        <v>32</v>
+      </c>
+      <c r="Q53" s="26">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:17">
+      <c r="B54" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C54" s="3">
+        <f>C19*C20*C21</f>
+        <v>5913</v>
+      </c>
+      <c r="N54" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="O54" s="49">
         <f>IF(O34=1,O16,O15*POWER(2,2)/2)</f>
         <v>16</v>
       </c>
-      <c r="Q53" s="30">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="2:17">
-      <c r="B54" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="3">
-        <f>C19*C20*C21</f>
-        <v>1</v>
-      </c>
-      <c r="N54" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="O54" s="55">
+      <c r="Q54" s="26">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:17">
+      <c r="B55" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="32">
+        <f>CEILING(C54,I11)</f>
+        <v>5916</v>
+      </c>
+      <c r="N55" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="O55" s="51">
         <f>O18</f>
         <v>8</v>
       </c>
-      <c r="Q54" s="30">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="2:17">
-      <c r="B55" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C55" s="36">
-        <f>CEILING(C54,I11)</f>
-        <v>4</v>
-      </c>
-      <c r="N55" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="O55" s="55">
-        <f>IF(O34=1,0,O27)</f>
-        <v>8</v>
-      </c>
-      <c r="Q55" s="30">
+      <c r="Q55" s="26">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
     </row>
     <row r="56" spans="2:17">
-      <c r="B56" s="78" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56" s="81">
+      <c r="B56" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="77">
         <f>C55/I11</f>
-        <v>1</v>
-      </c>
-      <c r="N56" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="O56" s="55">
-        <f>IF(O33=1, O55,0)</f>
-        <v>8</v>
-      </c>
-      <c r="Q56" s="30">
+        <v>1479</v>
+      </c>
+      <c r="N56" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="O56" s="51">
+        <f>O27</f>
+        <v>16</v>
+      </c>
+      <c r="Q56" s="26">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
     </row>
     <row r="57" spans="2:17">
       <c r="B57" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C57" s="80">
+        <v>117</v>
+      </c>
+      <c r="C57" s="76">
         <f>C56/I13</f>
-        <v>6.6666666666666664E-4</v>
-      </c>
-      <c r="N57" s="53" t="s">
-        <v>168</v>
-      </c>
-      <c r="O57" s="55">
-        <f>O52+O54+O55+O56</f>
-        <v>40</v>
-      </c>
-      <c r="Q57" s="30">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="N57" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="O57" s="51">
+        <f>IF(O33=1,O27,0)</f>
+        <v>16</v>
+      </c>
+      <c r="Q57" s="26">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
     </row>
     <row r="58" spans="2:17">
       <c r="B58" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C58" s="42">
+        <v>116</v>
+      </c>
+      <c r="C58" s="38">
         <f>C57/0.2</f>
-        <v>3.3333333333333331E-3</v>
-      </c>
-      <c r="Q58" s="30">
+        <v>4.93</v>
+      </c>
+      <c r="N58" s="49" t="s">
+        <v>169</v>
+      </c>
+      <c r="O58" s="51" t="str">
+        <f>IF(O43=0,O53+O55+O56+O57,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="Q58" s="26">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
     </row>
     <row r="59" spans="2:17">
-      <c r="N59" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="O59" s="53">
-        <v>26</v>
-      </c>
-      <c r="Q59" s="30">
+      <c r="Q59" s="26">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
     </row>
     <row r="60" spans="2:17">
       <c r="B60" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C60" s="3">
         <f>IF(O37=1,CEILING(C79,C23)/C23,IF(O35=0,C79,CEILING(C79,64)/64))</f>
-        <v>262144</v>
-      </c>
-      <c r="N60" s="53" t="s">
-        <v>129</v>
-      </c>
-      <c r="O60" s="55">
-        <f>POWER(2,O59)</f>
-        <v>67108864</v>
-      </c>
-      <c r="Q60" s="30">
+        <v>504000</v>
+      </c>
+      <c r="N60" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="O60" s="49">
+        <v>26</v>
+      </c>
+      <c r="Q60" s="26">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
     <row r="61" spans="2:17">
       <c r="B61" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C61" s="3">
         <f>C77*(1+O37)</f>
-        <v>30720</v>
-      </c>
-      <c r="Q61" s="30">
+        <v>18432</v>
+      </c>
+      <c r="N61" s="49" t="s">
+        <v>165</v>
+      </c>
+      <c r="O61" s="51">
+        <f>POWER(2,O60)</f>
+        <v>67108864</v>
+      </c>
+      <c r="Q61" s="26">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
     <row r="62" spans="2:17">
       <c r="B62" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C62" s="43">
+        <v>76</v>
+      </c>
+      <c r="C62" s="39">
         <f>MAX(C60/C61,C61/C60)</f>
-        <v>8.5333333333333332</v>
-      </c>
-      <c r="N62" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="O62" s="53">
+        <v>27.34375</v>
+      </c>
+      <c r="Q62" s="26">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17">
+      <c r="B63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C63" s="3">
+        <f>2*C60*C61*O29+C61*C61*O30</f>
+        <v>3681386496</v>
+      </c>
+      <c r="N63" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="O63" s="49">
         <f>IF(C17=L23,0.0000000596,0.000000000000000111)</f>
         <v>5.9599999999999998E-8</v>
       </c>
-      <c r="Q62" s="30">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="2:17">
-      <c r="B63" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C63" s="3">
-        <f>2*C60*C61*O29+C61*C61*O30</f>
-        <v>5788139520</v>
-      </c>
-      <c r="Q63" s="30">
+      <c r="Q63" s="26">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
     </row>
     <row r="64" spans="2:17">
-      <c r="N64" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="O64" s="53">
-        <f>IF(O43=0,O57,O54+O30)</f>
-        <v>12</v>
-      </c>
-      <c r="Q64" s="30">
+      <c r="Q64" s="26">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:17">
       <c r="B65" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C65" s="3">
+        <v>78</v>
+      </c>
+      <c r="C65" s="3" t="str">
         <f>IF(O38=1,CEILING(CEILING(CEILING(C19+1,2)/2,C21)/C21,C24)/C24,"N/A")</f>
-        <v>1</v>
-      </c>
-      <c r="N65" s="53" t="s">
-        <v>164</v>
-      </c>
-      <c r="O65" s="53">
-        <f>IF(O43=0,1,POWER(2,O40))</f>
-        <v>4</v>
-      </c>
-      <c r="Q65" s="30">
+        <v>N/A</v>
+      </c>
+      <c r="N65" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="O65" s="49">
+        <f>IF(O43=0,1,O52)</f>
+        <v>8</v>
+      </c>
+      <c r="Q65" s="26">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:17">
       <c r="B66" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C66" s="3" t="str">
+        <v>79</v>
+      </c>
+      <c r="C66" s="3">
         <f>IF(O39=1,CEILING((C19+1)*(C19+2),C21*C24)/(C21*C24),"N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="Q66" s="30">
+        <v>69</v>
+      </c>
+      <c r="N66" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="O66" s="49">
+        <f>IF(O43=0,O58,O55+O30)</f>
+        <v>12</v>
+      </c>
+      <c r="Q66" s="26">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:17">
       <c r="B67" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C67" s="3" t="str">
+        <v>80</v>
+      </c>
+      <c r="C67" s="3">
         <f>IF(O39=1,C84,"N/A")</f>
-        <v>N/A</v>
-      </c>
-      <c r="Q67" s="30">
-        <f t="shared" ref="Q67:Q90" si="7">Q66+1</f>
+        <v>24</v>
+      </c>
+      <c r="N67" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="O67" s="49">
+        <f>O52/O65</f>
+        <v>1</v>
+      </c>
+      <c r="Q67" s="26">
+        <f t="shared" ref="Q67:Q90" si="2">Q66+1</f>
         <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:17">
-      <c r="D68" s="29"/>
-      <c r="Q68" s="30">
-        <f t="shared" si="7"/>
+      <c r="D68" s="25"/>
+      <c r="Q68" s="26">
+        <f t="shared" si="2"/>
         <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:17">
       <c r="B69" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C69" s="46">
+        <v>87</v>
+      </c>
+      <c r="C69" s="42">
         <f>IF(O38=1,C14*C13*C13/2,C14*C13*C13*C13/6)</f>
-        <v>123695058124800</v>
-      </c>
-      <c r="Q69" s="30">
-        <f t="shared" si="7"/>
+        <v>5.1157022628460364E+22</v>
+      </c>
+      <c r="Q69" s="26">
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:17">
-      <c r="B70" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="C70" s="57">
-        <f>I21*1000000000000000</f>
-        <v>1.6875E+18</v>
-      </c>
-      <c r="Q70" s="30">
-        <f t="shared" si="7"/>
+      <c r="B70" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C70" s="53">
+        <f>I22*1000000000000000</f>
+        <v>8.4375E+17</v>
+      </c>
+      <c r="Q70" s="26">
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:17">
-      <c r="B71" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="C71" s="58">
-        <f>1.75/82</f>
-        <v>2.1341463414634148E-2</v>
-      </c>
-      <c r="Q71" s="30">
-        <f t="shared" si="7"/>
+      <c r="B71" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="54">
+        <f>C47</f>
+        <v>0.38411625073506284</v>
+      </c>
+      <c r="Q71" s="26">
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:17">
-      <c r="A72" s="104" t="s">
-        <v>124</v>
+      <c r="A72" s="99" t="s">
+        <v>118</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C72" s="79">
+        <v>108</v>
+      </c>
+      <c r="C72" s="75">
         <f>C70*C71</f>
-        <v>3.6013719512195124E+16</v>
-      </c>
-      <c r="Q72" s="30">
-        <f t="shared" si="7"/>
+        <v>3.2409808655770925E+17</v>
+      </c>
+      <c r="Q72" s="26">
+        <f t="shared" si="2"/>
         <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:17">
-      <c r="A73" s="105"/>
-      <c r="B73" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="C73" s="89">
+      <c r="A73" s="100"/>
+      <c r="B73" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" s="114">
         <f>C69/C72/3600*I13</f>
-        <v>1.4311103726608251E-3</v>
-      </c>
-      <c r="E73" s="51"/>
-      <c r="Q73" s="30">
-        <f t="shared" si="7"/>
+        <v>65768.441651679954</v>
+      </c>
+      <c r="E73" s="47"/>
+      <c r="Q73" s="26">
+        <f t="shared" si="2"/>
         <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:17">
       <c r="B74" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C74" s="80" t="e">
-        <f>C73/I19</f>
+        <v>111</v>
+      </c>
+      <c r="C74" s="76" t="e">
+        <f>C73/I20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q74" s="30">
-        <f t="shared" si="7"/>
+      <c r="Q74" s="26">
+        <f t="shared" si="2"/>
         <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:17">
       <c r="C75" s="1"/>
-      <c r="G75" s="52"/>
-      <c r="Q75" s="30">
-        <f t="shared" si="7"/>
+      <c r="G75" s="48"/>
+      <c r="Q75" s="26">
+        <f t="shared" si="2"/>
         <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:17">
-      <c r="Q76" s="30">
-        <f t="shared" si="7"/>
+      <c r="A76" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q76" s="26">
+        <f t="shared" si="2"/>
         <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:17">
       <c r="A77" s="10"/>
       <c r="B77" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C77" s="3">
         <f>CEILING(CEILING(C13,C19)/C19,IF(O39=1,6,1))</f>
-        <v>15360</v>
-      </c>
-      <c r="D77" s="29"/>
-      <c r="Q77" s="30">
-        <f t="shared" si="7"/>
+        <v>9216</v>
+      </c>
+      <c r="D77" s="25"/>
+      <c r="Q77" s="26">
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:17">
       <c r="B78" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C78" s="3">
         <f>IF(AND(O37=0,O39=0),C77,IF(O37=0,CEILING(C77,6),IF(O39=0,CEILING(C77,4),CEILING(C77,24))))</f>
-        <v>15360</v>
-      </c>
-      <c r="Q78" s="30">
-        <f t="shared" si="7"/>
+        <v>9216</v>
+      </c>
+      <c r="Q78" s="26">
+        <f t="shared" si="2"/>
         <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:17">
       <c r="B79" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C79" s="3">
         <f>CEILING(C14,C20)/C20</f>
-        <v>1048576</v>
-      </c>
-      <c r="Q79" s="30">
-        <f t="shared" si="7"/>
+        <v>1008000</v>
+      </c>
+      <c r="Q79" s="26">
+        <f t="shared" si="2"/>
         <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:17">
-      <c r="Q80" s="30">
-        <f t="shared" si="7"/>
+      <c r="Q80" s="26">
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="2:17">
       <c r="B81" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C81" s="3">
         <f>CEILING(C79*O51,O12)/O12</f>
-        <v>262144</v>
-      </c>
-      <c r="Q81" s="30">
-        <f t="shared" si="7"/>
+        <v>252000</v>
+      </c>
+      <c r="Q81" s="26">
+        <f t="shared" si="2"/>
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="2:17">
       <c r="B82" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C82" s="3">
         <f>C81*C77</f>
-        <v>4026531840</v>
-      </c>
-      <c r="Q82" s="30">
-        <f t="shared" si="7"/>
+        <v>2322432000</v>
+      </c>
+      <c r="Q82" s="26">
+        <f t="shared" si="2"/>
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="2:17">
       <c r="B83" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C83" s="3">
-        <f>O53*C77*C77</f>
-        <v>3774873600</v>
-      </c>
-      <c r="Q83" s="30">
-        <f t="shared" si="7"/>
+        <f>O54*C77*C77</f>
+        <v>1358954496</v>
+      </c>
+      <c r="Q83" s="26">
+        <f t="shared" si="2"/>
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="2:17">
       <c r="B84" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C84" s="3">
         <f>CEILING(C77,6*C25)/(6*C25)</f>
-        <v>2560</v>
-      </c>
-      <c r="Q84" s="30">
-        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+      <c r="Q84" s="26">
+        <f t="shared" si="2"/>
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
-      <c r="B85" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C85" s="3">
-        <f>O64*C77*C77*C84</f>
-        <v>7247757312000</v>
-      </c>
-      <c r="Q85" s="30">
-        <f t="shared" si="7"/>
+    <row r="85" spans="2:17">
+      <c r="B85" s="112" t="s">
+        <v>158</v>
+      </c>
+      <c r="C85" s="113">
+        <f>O66*C77*C77*C84</f>
+        <v>24461180928</v>
+      </c>
+      <c r="E85" s="115" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q85" s="26">
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="2:17">
       <c r="B86" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C86" s="3">
+        <f>C77*O16*(1+O32)*(1+O33)</f>
+        <v>73728</v>
+      </c>
+      <c r="Q86" s="26">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="2:17">
+      <c r="B87" s="112" t="s">
+        <v>68</v>
+      </c>
+      <c r="C87" s="113" t="str">
+        <f>IF(O38=1,C83*C65/C26,"N/A")</f>
+        <v>N/A</v>
+      </c>
+      <c r="E87" s="115" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q87" s="26">
+        <f t="shared" si="2"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="2:17">
+      <c r="B88" s="112" t="s">
         <v>69</v>
       </c>
-      <c r="C86" s="3">
-        <f>C77*O16*IF(O38=1,1,(1+O32)*(1+O33))</f>
-        <v>61440</v>
-      </c>
-      <c r="Q86" s="30">
-        <f t="shared" si="7"/>
-        <v>86</v>
-      </c>
-    </row>
-    <row r="87" spans="1:17">
-      <c r="B87" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C87" s="3">
-        <f>IF(O38=1,C83*C65/C26,"N/A")</f>
-        <v>3774873.6000000001</v>
-      </c>
-      <c r="Q87" s="30">
-        <f t="shared" si="7"/>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="88" spans="1:17">
-      <c r="B88" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C88" s="3" t="str">
+      <c r="C88" s="113">
         <f>IF(O39=1,C85*C66/C26,"N/A")</f>
+        <v>4219553710.0799999</v>
+      </c>
+      <c r="E88" s="115" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q88" s="26">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="2:17">
+      <c r="B89" s="112" t="s">
+        <v>67</v>
+      </c>
+      <c r="C89" s="113">
+        <f>IF(O38=1,C87,C88)</f>
+        <v>4219553710.0799999</v>
+      </c>
+      <c r="E89" s="115" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q89" s="26">
+        <f t="shared" si="2"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="2:17">
+      <c r="B90" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90" s="3" t="str">
+        <f>IF(O38=1,C65*C78*C78,"N/A")</f>
         <v>N/A</v>
       </c>
-      <c r="Q88" s="30">
-        <f t="shared" si="7"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="89" spans="1:17">
-      <c r="B89" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C89" s="3">
-        <f>IF(O38=1,C87,C88)</f>
-        <v>3774873.6000000001</v>
-      </c>
-      <c r="Q89" s="30">
-        <f t="shared" si="7"/>
-        <v>89</v>
-      </c>
-    </row>
-    <row r="90" spans="1:17">
-      <c r="B90" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C90" s="3">
-        <f>IF(O38=1,C65*C78*C78,"N/A")</f>
-        <v>235929600</v>
-      </c>
-      <c r="Q90" s="30">
-        <f t="shared" si="7"/>
+      <c r="Q90" s="26">
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="2:17">
       <c r="B91" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C91" s="3">
+        <f>IF(O39=1,C84*C78*C78*C66,"N/A")</f>
+        <v>140651790336</v>
+      </c>
+    </row>
+    <row r="92" spans="2:17">
+      <c r="B92" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="C91" s="3" t="str">
-        <f>IF(O39=1,C84*C78*C78,"N/A")</f>
-        <v>N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="1:17">
-      <c r="B92" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="C92" s="3">
         <f>IF(O38=1,C90,C91)</f>
-        <v>235929600</v>
-      </c>
-    </row>
-    <row r="93" spans="1:17">
+        <v>140651790336</v>
+      </c>
+    </row>
+    <row r="93" spans="2:17">
       <c r="B93" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C93" s="3">
-        <f>IF(O43=0,B92*(O52+O54),C92*O65*(O64+O54))/C26</f>
-        <v>18874368</v>
-      </c>
-    </row>
-    <row r="96" spans="1:17">
-      <c r="A96" s="92" t="s">
-        <v>151</v>
-      </c>
-      <c r="E96" s="94" t="s">
-        <v>146</v>
-      </c>
-      <c r="F96" s="94" t="s">
-        <v>147</v>
-      </c>
-      <c r="G96" s="94" t="s">
+        <f>C92*O65</f>
+        <v>1125214322688</v>
+      </c>
+    </row>
+    <row r="94" spans="2:17">
+      <c r="B94" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C94" s="3">
+        <f>C93/C26</f>
+        <v>2813035806.7199998</v>
+      </c>
+    </row>
+    <row r="95" spans="2:17">
+      <c r="B95" s="112" t="s">
+        <v>159</v>
+      </c>
+      <c r="C95" s="113">
+        <f>IF(O43=0,B92*(O53+O55),C92*O65*(O66+O55))/C26</f>
+        <v>56260716134.400002</v>
+      </c>
+      <c r="E95" s="115" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17">
+      <c r="A98" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="F98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+    </row>
+    <row r="99" spans="1:17">
+      <c r="A99" s="87"/>
+      <c r="E99" s="89" t="s">
+        <v>138</v>
+      </c>
+      <c r="F99" s="89" t="s">
+        <v>139</v>
+      </c>
+      <c r="G99" s="89" t="s">
+        <v>140</v>
+      </c>
+      <c r="H99" s="89" t="s">
         <v>148</v>
       </c>
-      <c r="H96" s="94" t="s">
-        <v>157</v>
-      </c>
-      <c r="I96" s="94" t="s">
-        <v>158</v>
-      </c>
-      <c r="J96" s="92"/>
-      <c r="K96" s="94" t="s">
+      <c r="I99" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="L96" s="94" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12">
-      <c r="A97" s="90" t="s">
-        <v>145</v>
-      </c>
-      <c r="E97" s="2">
+      <c r="J99" s="87"/>
+      <c r="K99" s="89" t="s">
+        <v>141</v>
+      </c>
+      <c r="L99" s="89" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17">
+      <c r="A100" s="85" t="s">
+        <v>137</v>
+      </c>
+      <c r="E100" s="2">
         <v>4</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F100" s="2">
         <v>3</v>
       </c>
-      <c r="G97" s="2"/>
-      <c r="H97" s="3">
+      <c r="G100" s="2"/>
+      <c r="H100" s="3">
         <f>3 * C86</f>
-        <v>184320</v>
-      </c>
-      <c r="I97" s="3">
-        <f>H97</f>
-        <v>184320</v>
-      </c>
-      <c r="J97" s="91"/>
-      <c r="K97" s="3">
-        <f t="shared" ref="K97:K103" si="8">E97*C$82+F97*C$82+G97*C$83+H97</f>
-        <v>28185907200</v>
-      </c>
-      <c r="L97" s="3">
-        <f t="shared" ref="L97:L103" si="9">F97*C$82+G97*C$83+I97</f>
-        <v>12079779840</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12">
-      <c r="A98" s="90" t="s">
-        <v>152</v>
-      </c>
-      <c r="E98" s="2"/>
-      <c r="G98" s="2">
+        <v>221184</v>
+      </c>
+      <c r="I100" s="3">
+        <f>H100</f>
+        <v>221184</v>
+      </c>
+      <c r="J100" s="86"/>
+      <c r="K100" s="3">
+        <f>IF(O38=0,E100*C$82+F100*C$82+G100*C$83+H100,0)</f>
+        <v>16257245184</v>
+      </c>
+      <c r="L100" s="3">
+        <f>IF(O38=0,F100*C$82+G100*C$83+I100,0)</f>
+        <v>6967517184</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17">
+      <c r="A101" s="85" t="s">
+        <v>143</v>
+      </c>
+      <c r="E101" s="2"/>
+      <c r="G101" s="2">
         <f>2*(O32*1+1)+O34*3</f>
         <v>2</v>
       </c>
-      <c r="H98" s="3">
+      <c r="H101" s="3">
         <f>2*(C81*IF(O44=1,1,C78))</f>
-        <v>524288</v>
-      </c>
-      <c r="I98" s="3">
-        <f>H98</f>
-        <v>524288</v>
-      </c>
-      <c r="J98" s="91"/>
-      <c r="K98" s="3">
-        <f t="shared" si="8"/>
-        <v>7550271488</v>
-      </c>
-      <c r="L98" s="3">
-        <f t="shared" si="9"/>
-        <v>7550271488</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12">
-      <c r="A99" s="90" t="s">
-        <v>153</v>
-      </c>
-      <c r="E99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="3">
-        <f>IF(O45=1,C78*C78*4*(4+8),0)</f>
-        <v>11324620800</v>
-      </c>
-      <c r="I99" s="3">
-        <f>H99</f>
-        <v>11324620800</v>
-      </c>
-      <c r="J99" s="91"/>
-      <c r="K99" s="3">
-        <f t="shared" si="8"/>
-        <v>11324620800</v>
-      </c>
-      <c r="L99" s="3">
-        <f t="shared" si="9"/>
-        <v>11324620800</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12">
-      <c r="A100" s="90" t="s">
-        <v>156</v>
-      </c>
-      <c r="E100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="3">
-        <f>O37*(2*2*C78*C79*O29/C23+O46*C78*2*4)</f>
-        <v>2013388800</v>
-      </c>
-      <c r="J100" s="91"/>
-      <c r="K100" s="3">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="L100" s="3">
-        <f t="shared" si="9"/>
-        <v>2013388800</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12">
-      <c r="A101" s="90" t="s">
-        <v>159</v>
-      </c>
-      <c r="E101" s="2">
-        <v>1</v>
-      </c>
-      <c r="G101" s="2"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="91"/>
+        <v>504000</v>
+      </c>
+      <c r="I101" s="3">
+        <f>H101</f>
+        <v>504000</v>
+      </c>
+      <c r="J101" s="86"/>
       <c r="K101" s="3">
-        <f t="shared" si="8"/>
-        <v>4026531840</v>
+        <f>IF(O38=0,E101*C$82+F101*C$82+G101*C$83+H101,0)</f>
+        <v>2718412992</v>
       </c>
       <c r="L101" s="3">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12">
-      <c r="A102" s="90" t="s">
-        <v>160</v>
-      </c>
+        <f>IF(O38=0,F101*C$82+G101*C$83+I101,0)</f>
+        <v>2718412992</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17">
+      <c r="A102" s="85" t="s">
+        <v>144</v>
+      </c>
+      <c r="E102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="3">
-        <f>C93+IF(O47=1,0,C92*(O55+O56))</f>
-        <v>18874368</v>
-      </c>
-      <c r="I102" s="3"/>
-      <c r="J102" s="91"/>
+        <f>IF(O45=1,C78*C78*4*(4+8),0)</f>
+        <v>4076863488</v>
+      </c>
+      <c r="I102" s="3">
+        <f>H102</f>
+        <v>4076863488</v>
+      </c>
+      <c r="J102" s="86"/>
       <c r="K102" s="3">
-        <f t="shared" si="8"/>
-        <v>18874368</v>
+        <f t="shared" ref="K102:K105" si="3">E102*C$82+F102*C$82+G102*C$83+H102</f>
+        <v>4076863488</v>
       </c>
       <c r="L102" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="L102:L105" si="4">F102*C$82+G102*C$83+I102</f>
+        <v>4076863488</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17">
+      <c r="A103" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="E103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3">
+        <f>O37*(2*2*C78*C79*O29/C23+O46*C78*2*4)</f>
+        <v>2322432000</v>
+      </c>
+      <c r="J103" s="86"/>
+      <c r="K103" s="3">
+        <f>E103*C$82+F103*C$82+G103*C$83+H103</f>
         <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12">
-      <c r="A103" s="93" t="s">
-        <v>174</v>
-      </c>
-      <c r="F103" s="2">
-        <v>3</v>
-      </c>
-      <c r="G103" s="2">
-        <f>2+O32*1</f>
-        <v>2</v>
-      </c>
-      <c r="H103" s="3">
-        <f>3 * C86</f>
-        <v>184320</v>
-      </c>
-      <c r="I103" s="3">
-        <f>H103</f>
-        <v>184320</v>
-      </c>
-      <c r="J103" s="91"/>
-      <c r="K103" s="3">
-        <f t="shared" si="8"/>
-        <v>19629527040</v>
       </c>
       <c r="L103" s="3">
         <f>F103*C$82+G103*C$83+I103</f>
-        <v>19629527040</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12">
-      <c r="A104" s="90"/>
+        <v>2322432000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17">
+      <c r="A104" s="85" t="s">
+        <v>150</v>
+      </c>
+      <c r="E104" s="2">
+        <v>1</v>
+      </c>
       <c r="G104" s="2"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="91"/>
-      <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
-    </row>
-    <row r="105" spans="1:12">
-      <c r="A105" s="90"/>
+      <c r="J104" s="86"/>
+      <c r="K104" s="3">
+        <f t="shared" si="3"/>
+        <v>2322432000</v>
+      </c>
+      <c r="L104" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17">
+      <c r="A105" s="85" t="s">
+        <v>151</v>
+      </c>
       <c r="G105" s="2"/>
-      <c r="H105" s="3"/>
+      <c r="H105" s="3">
+        <f>C94*O66+IF(O47=1,0,C92*(O56+O57))</f>
+        <v>33756429680.639999</v>
+      </c>
       <c r="I105" s="3"/>
-      <c r="J105" s="91"/>
-      <c r="K105" s="3"/>
-      <c r="L105" s="3"/>
-    </row>
-    <row r="106" spans="1:12">
-      <c r="A106" s="90"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="3"/>
-      <c r="J106" s="91"/>
-      <c r="K106" s="3"/>
-      <c r="L106" s="3"/>
-    </row>
-    <row r="107" spans="1:12">
-      <c r="A107" s="90"/>
+      <c r="J105" s="86"/>
+      <c r="K105" s="3">
+        <f t="shared" si="3"/>
+        <v>33756429680.639999</v>
+      </c>
+      <c r="L105" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17">
+      <c r="A106" s="88" t="s">
+        <v>160</v>
+      </c>
+      <c r="F106" s="2">
+        <v>3</v>
+      </c>
+      <c r="G106" s="2">
+        <f>2+O32*1</f>
+        <v>2</v>
+      </c>
+      <c r="H106" s="3">
+        <f>3 * C86</f>
+        <v>221184</v>
+      </c>
+      <c r="I106" s="3">
+        <f>H106</f>
+        <v>221184</v>
+      </c>
+      <c r="J106" s="86"/>
+      <c r="K106" s="3">
+        <f>IF(O38=1,E106*C$82+F106*C$82+G106*C$83+H106,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L106" s="3">
+        <f>IF(O38=1,F106*C$82+G106*C$83+I106,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17">
+      <c r="A107" s="85"/>
       <c r="G107" s="2"/>
+      <c r="H107" s="3"/>
       <c r="I107" s="3"/>
-      <c r="J107" s="91"/>
+      <c r="J107" s="86"/>
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12">
-      <c r="A108" s="90"/>
-      <c r="G108" s="2"/>
-      <c r="I108" s="3"/>
-      <c r="J108" s="91"/>
-      <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
-    </row>
-    <row r="109" spans="1:12">
-      <c r="A109" s="90"/>
+    <row r="108" spans="1:17" s="87" customFormat="1">
+      <c r="A108" s="101" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" s="89"/>
+      <c r="C108" s="102"/>
+      <c r="F108" s="89"/>
+      <c r="G108" s="89"/>
+      <c r="H108" s="89"/>
+      <c r="I108" s="102"/>
+      <c r="J108" s="103"/>
+      <c r="K108" s="102">
+        <f>SUM(K100:K106)</f>
+        <v>59131383344.639999</v>
+      </c>
+      <c r="L108" s="102">
+        <f>SUM(L100:L106)</f>
+        <v>16085225664</v>
+      </c>
+      <c r="N108" s="104"/>
+      <c r="O108" s="104"/>
+      <c r="Q108" s="89"/>
+    </row>
+    <row r="109" spans="1:17">
+      <c r="A109" s="85"/>
       <c r="G109" s="2"/>
       <c r="I109" s="3"/>
-      <c r="J109" s="91"/>
+      <c r="J109" s="86"/>
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12">
-      <c r="A110" s="90"/>
+    <row r="110" spans="1:17">
+      <c r="A110" s="85"/>
       <c r="G110" s="2"/>
       <c r="I110" s="3"/>
-      <c r="J110" s="91"/>
+      <c r="J110" s="86"/>
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12">
-      <c r="A111" s="90"/>
+    <row r="111" spans="1:17">
+      <c r="A111" s="85"/>
       <c r="G111" s="2"/>
       <c r="I111" s="3"/>
-      <c r="J111" s="91"/>
+      <c r="J111" s="86"/>
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:17">
+      <c r="A112" s="85"/>
       <c r="G112" s="2"/>
       <c r="I112" s="3"/>
-      <c r="J112" s="91"/>
+      <c r="J112" s="86"/>
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
+    </row>
+    <row r="113" spans="7:12">
+      <c r="G113" s="2"/>
+      <c r="I113" s="3"/>
+      <c r="J113" s="86"/>
+      <c r="K113" s="3"/>
+      <c r="L113" s="3"/>
+    </row>
+    <row r="114" spans="7:12">
+      <c r="K114" s="3"/>
+    </row>
+    <row r="115" spans="7:12">
+      <c r="K115" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4937,18 +5036,6 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A72:A73"/>
   </mergeCells>
-  <conditionalFormatting sqref="C45">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="$I$16 * 0.95"/>
-        <cfvo type="num" val="$I$16"/>
-        <color rgb="FF00FF01"/>
-        <color rgb="FFFFFE00"/>
-        <color rgb="FFFF7F82"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C56">
     <cfRule type="colorScale" priority="14">
       <colorScale>
@@ -4961,7 +5048,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C45">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -5129,6 +5216,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="$I$18 * 0.95"/>
+        <cfvo type="num" val="$I$18"/>
+        <color rgb="FF00FF01"/>
+        <color rgb="FFFFFE00"/>
+        <color rgb="FFFF7F82"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="9">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{5DA3BF6A-F4AE-C741-BD81-2AE26555EC93}">
       <formula1>$L$9:$L$10</formula1>

</xml_diff>